<commit_message>
Ressourcenkalkulation und Excelformaln im Netzplan.
</commit_message>
<xml_diff>
--- a/Online_Shop.Projekt.xlsx
+++ b/Online_Shop.Projekt.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="58">
   <si>
     <t xml:space="preserve">Beispiel: Funktionsorientierter Projektstrukturplan</t>
   </si>
@@ -171,7 +171,16 @@
     <t xml:space="preserve">Aufwand</t>
   </si>
   <si>
+    <t xml:space="preserve">Personen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kapazität</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.1.1, 1.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">1.1.2, 1.1.3</t>
@@ -193,13 +202,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="166" formatCode="@"/>
-    <numFmt numFmtId="167" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="0.00\ %"/>
+    <numFmt numFmtId="168" formatCode="0\ %"/>
+    <numFmt numFmtId="169" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -224,6 +235,7 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -231,7 +243,14 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -321,7 +340,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -345,8 +364,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -355,7 +377,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -379,15 +401,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,7 +449,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -440,6 +470,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -459,19 +493,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -495,15 +529,31 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="KritischerPfad" xfId="20"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="1"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -558,7 +608,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -589,7 +639,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8109360" y="325080"/>
+          <a:off x="8118360" y="325080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -630,8 +680,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5393520" y="479520"/>
-          <a:ext cx="5430600" cy="0"/>
+          <a:off x="5399280" y="479520"/>
+          <a:ext cx="5438160" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -671,7 +721,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5412240" y="488160"/>
+          <a:off x="5418720" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -712,7 +762,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5413320" y="488160"/>
+          <a:off x="5419800" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -753,7 +803,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8120160" y="488160"/>
+          <a:off x="8130600" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -794,7 +844,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10827000" y="488160"/>
+          <a:off x="10841040" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -835,7 +885,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5413320" y="1122120"/>
+          <a:off x="5419800" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -876,7 +926,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5413320" y="1609560"/>
+          <a:off x="5419800" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -917,7 +967,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5413320" y="2097720"/>
+          <a:off x="5419800" y="2097720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -958,7 +1008,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5413320" y="2584800"/>
+          <a:off x="5419800" y="2584800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -999,7 +1049,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8120160" y="1122120"/>
+          <a:off x="8130600" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1040,7 +1090,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8120160" y="1609560"/>
+          <a:off x="8130600" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1081,7 +1131,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8120160" y="2097720"/>
+          <a:off x="8130600" y="2097720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1122,7 +1172,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8120160" y="2584800"/>
+          <a:off x="8130600" y="2584800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1163,7 +1213,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8120160" y="3072240"/>
+          <a:off x="8130600" y="3072240"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1204,7 +1254,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8120160" y="3560400"/>
+          <a:off x="8130600" y="3560400"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1245,7 +1295,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8120160" y="4047480"/>
+          <a:off x="8130600" y="4047480"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1286,7 +1336,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8120160" y="4534920"/>
+          <a:off x="8130600" y="4534920"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1327,7 +1377,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8120160" y="5023080"/>
+          <a:off x="8130600" y="5023080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1368,7 +1418,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10827360" y="2097360"/>
+          <a:off x="10841400" y="2097360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1409,7 +1459,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10827360" y="1609560"/>
+          <a:off x="10841400" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1450,7 +1500,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10827360" y="1121760"/>
+          <a:off x="10841400" y="1121760"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1476,18 +1526,18 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1080</xdr:colOff>
+      <xdr:rowOff>151200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1496,7 +1546,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7107480" y="475560"/>
+          <a:off x="7113240" y="475920"/>
           <a:ext cx="535320" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1504,7 +1554,7 @@
         </a:prstGeom>
         <a:ln w="36000">
           <a:solidFill>
-            <a:srgbClr val="ff0000"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -1518,199 +1568,497 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>264960</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:rowOff>157320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>265320</xdr:colOff>
       <xdr:row>2</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8453160" y="482040"/>
+          <a:ext cx="541440" cy="5400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>253080</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>12960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>12960</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7359120" y="500040"/>
+          <a:ext cx="18000" cy="1950840"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>157320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>259560</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>157320</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7383600" y="2432880"/>
+          <a:ext cx="252360" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>1440</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>151200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>241200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9812160" y="475920"/>
+          <a:ext cx="1863000" cy="5400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>255960</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>270000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>5760</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11419200" y="491040"/>
+          <a:ext cx="284760" cy="2160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>264600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>264960</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name=""/>
+        <xdr:cNvPr id="28" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8452800" y="2433600"/>
+          <a:ext cx="541440" cy="5040"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>264240</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>258840</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>163080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8448120" y="481680"/>
-          <a:ext cx="541440" cy="6120"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>97920</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>155160</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name=""/>
+          <a:off x="9804960" y="2433600"/>
+          <a:ext cx="535680" cy="5040"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>255960</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>155160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>255960</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>162360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8714520" y="480240"/>
+          <a:ext cx="0" cy="982440"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>249480</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>254160</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>156240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="7359480" y="499680"/>
-          <a:ext cx="6480" cy="1950840"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+          <a:off x="8707680" y="1452240"/>
+          <a:ext cx="275400" cy="3960"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>255960</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>155520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>10800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9796320" y="1455840"/>
+          <a:ext cx="566280" cy="7200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>260640</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>155160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>9000</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>155160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12506400" y="480240"/>
+          <a:ext cx="559800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>261000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>138600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>156600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>259200</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name=""/>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7377840" y="2432160"/>
-          <a:ext cx="252360" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>720</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>240480</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="26" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9806400" y="475560"/>
-          <a:ext cx="1863000" cy="5400"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>255240</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>269280</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="11413440" y="490680"/>
-          <a:ext cx="284760" cy="2160"/>
+          <a:off x="10072080" y="1926720"/>
+          <a:ext cx="10080" cy="505440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="36000">
           <a:solidFill>
-            <a:srgbClr val="ff0000"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -1724,389 +2072,100 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>264600</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="8447760" y="2432520"/>
-          <a:ext cx="541440" cy="6120"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>264240</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>258840</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9799920" y="2432520"/>
-          <a:ext cx="535680" cy="6120"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>255240</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>255240</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8708760" y="480240"/>
-          <a:ext cx="0" cy="982800"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>248760</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>253440</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="8701920" y="1451880"/>
-          <a:ext cx="275400" cy="3960"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>255600</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>10440</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9790920" y="1455840"/>
-          <a:ext cx="566280" cy="7200"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>260280</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>8640</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12501000" y="480240"/>
-          <a:ext cx="559800" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>260640</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>270720</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name=""/>
+      <xdr:rowOff>152640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>253440</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>157320</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10071360" y="1940400"/>
+          <a:ext cx="1345320" cy="4680"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>259560</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>105840</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>22320</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10066680" y="1926720"/>
-          <a:ext cx="10080" cy="505440"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>259920</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>252720</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="10065600" y="1940040"/>
-          <a:ext cx="1345320" cy="4680"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>259200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>270720</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="11417760" y="592920"/>
+          <a:off x="11423160" y="593280"/>
           <a:ext cx="11520" cy="1379520"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>7920</xdr:colOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2117,7 +2176,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11158920" y="1463040"/>
+          <a:off x="11164320" y="1463040"/>
           <a:ext cx="278280" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2125,7 +2184,7 @@
         </a:prstGeom>
         <a:ln w="36000">
           <a:solidFill>
-            <a:srgbClr val="ff0000"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -2139,15 +2198,15 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>36</xdr:col>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
       <xdr:colOff>8640</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>153360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>27360</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>153360</xdr:rowOff>
@@ -2159,15 +2218,15 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13872240" y="478440"/>
-          <a:ext cx="559800" cy="0"/>
+          <a:off x="13877640" y="478440"/>
+          <a:ext cx="559440" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="36000">
           <a:solidFill>
-            <a:srgbClr val="ff0000"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -2181,16 +2240,16 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>268560</xdr:colOff>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>269280</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>43</xdr:col>
-      <xdr:colOff>12960</xdr:colOff>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>13680</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
@@ -2201,15 +2260,15 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15214320" y="478080"/>
-          <a:ext cx="555840" cy="3600"/>
+          <a:off x="15219720" y="478080"/>
+          <a:ext cx="556200" cy="3600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="36000">
           <a:solidFill>
-            <a:srgbClr val="ff0000"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -2223,35 +2282,203 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>46</xdr:col>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>49</xdr:col>
       <xdr:colOff>18720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>48</xdr:col>
+      <xdr:rowOff>157320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
       <xdr:colOff>6840</xdr:colOff>
       <xdr:row>2</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="16592760" y="482040"/>
+          <a:ext cx="529200" cy="5400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>249480</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>19080</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>153720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17904960" y="477360"/>
+          <a:ext cx="581400" cy="1080"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>249480</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>153720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>259920</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="19257840" y="478440"/>
+          <a:ext cx="551160" cy="9000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>63</xdr:col>
+      <xdr:colOff>269280</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>153720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>65</xdr:col>
+      <xdr:colOff>269640</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="20630160" y="478440"/>
+          <a:ext cx="541080" cy="9000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>259560</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>265680</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="16587360" y="481680"/>
-          <a:ext cx="528840" cy="6120"/>
+        <xdr:cNvPr id="44" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20890800" y="488160"/>
+          <a:ext cx="6120" cy="1950480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="36000">
           <a:solidFill>
-            <a:srgbClr val="ff0000"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -2265,287 +2492,121 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>50</xdr:col>
-      <xdr:colOff>248760</xdr:colOff>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>53</xdr:col>
-      <xdr:colOff>18360</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17899200" y="477000"/>
-          <a:ext cx="581400" cy="1080"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>249120</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>57</xdr:col>
-      <xdr:colOff>259200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="19252080" y="478080"/>
-          <a:ext cx="551160" cy="9720"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>60</xdr:col>
-      <xdr:colOff>268920</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>153360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>62</xdr:col>
-      <xdr:colOff>268920</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="20624400" y="478080"/>
-          <a:ext cx="541080" cy="9720"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>61</xdr:col>
+      <xdr:rowOff>157320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>258840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>61</xdr:col>
+      <xdr:rowOff>1080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8465400" y="482040"/>
+          <a:ext cx="252000" cy="6120"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>51480</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>215280</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>3240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="11429640" y="488160"/>
+          <a:ext cx="4680" cy="975240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>264960</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name=""/>
+      <xdr:rowOff>157320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>250560</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>163440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20885040" y="487800"/>
-          <a:ext cx="6120" cy="1950480"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>6480</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>258480</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="45" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8460000" y="481680"/>
-          <a:ext cx="252000" cy="6120"/>
+          <a:off x="11157840" y="2432520"/>
+          <a:ext cx="9723960" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="36000">
           <a:solidFill>
-            <a:srgbClr val="ff0000"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>50760</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>214560</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="11423160" y="487800"/>
-          <a:ext cx="6120" cy="975240"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="ff0000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="twoCell">
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>264240</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>61</xdr:col>
-      <xdr:colOff>270000</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11152440" y="2432160"/>
-          <a:ext cx="9744120" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2567,11 +2628,11 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="G:I D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.77"/>
   </cols>
@@ -3112,17 +3173,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BN17"/>
+  <dimension ref="A1:BQ17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB5" activeCellId="0" sqref="AB5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="G:I"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="3" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="8" style="0" width="3.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="1" max="8" min="7" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="1" max="9" min="9" style="20" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="11" style="0" width="3.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3134,13 +3198,22 @@
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3153,88 +3226,119 @@
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="23" t="n">
+      <c r="E2" s="23"/>
+      <c r="F2" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="I2" s="24" t="n">
+      <c r="H2" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="25" t="n">
+        <f aca="false">ROUND(G2/(H2*I2),0)</f>
+        <v>5</v>
+      </c>
+      <c r="L2" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="24" t="n">
+      <c r="M2" s="28"/>
+      <c r="N2" s="27" t="n">
+        <f aca="false">L2+L4</f>
         <v>5</v>
       </c>
-      <c r="N2" s="24" t="n">
+      <c r="Q2" s="27" t="n">
+        <f aca="false">N2</f>
         <v>5</v>
       </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="24" t="n">
+      <c r="R2" s="28"/>
+      <c r="S2" s="27" t="n">
+        <f aca="false">Q2+Q4</f>
         <v>6</v>
       </c>
-      <c r="S2" s="24" t="n">
+      <c r="V2" s="27" t="n">
+        <f aca="false">S2</f>
         <v>6</v>
       </c>
-      <c r="T2" s="25"/>
-      <c r="U2" s="24" t="n">
+      <c r="W2" s="28"/>
+      <c r="X2" s="27" t="n">
+        <f aca="false">V2+V4</f>
         <v>10</v>
       </c>
-      <c r="AC2" s="24" t="n">
+      <c r="AF2" s="27" t="n">
+        <f aca="false">MAX(X2,AC8,X14)</f>
         <v>16</v>
       </c>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="24" t="n">
+      <c r="AG2" s="28"/>
+      <c r="AH2" s="27" t="n">
+        <f aca="false">AF2+AF4</f>
         <v>18</v>
       </c>
-      <c r="AH2" s="24" t="n">
+      <c r="AK2" s="27" t="n">
+        <f aca="false">AH2</f>
         <v>18</v>
       </c>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="24" t="n">
+      <c r="AL2" s="28"/>
+      <c r="AM2" s="27" t="n">
+        <f aca="false">AK2+AK4</f>
         <v>20</v>
       </c>
-      <c r="AM2" s="24" t="n">
+      <c r="AP2" s="27" t="n">
+        <f aca="false">AM2</f>
         <v>20</v>
       </c>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="24" t="n">
+      <c r="AQ2" s="28"/>
+      <c r="AR2" s="27" t="n">
+        <f aca="false">AP2+AP4</f>
         <v>22</v>
       </c>
-      <c r="AR2" s="24" t="n">
+      <c r="AU2" s="27" t="n">
+        <f aca="false">AR2</f>
         <v>22</v>
       </c>
-      <c r="AS2" s="25"/>
-      <c r="AT2" s="24" t="n">
+      <c r="AV2" s="28"/>
+      <c r="AW2" s="27" t="n">
+        <f aca="false">AU2+AU4</f>
         <v>25</v>
       </c>
-      <c r="AW2" s="24" t="n">
+      <c r="AZ2" s="27" t="n">
+        <f aca="false">AW2</f>
         <v>25</v>
       </c>
-      <c r="AX2" s="25"/>
-      <c r="AY2" s="24" t="n">
+      <c r="BA2" s="28"/>
+      <c r="BB2" s="27" t="n">
+        <f aca="false">AZ2+AZ4</f>
         <v>28</v>
       </c>
-      <c r="BB2" s="24" t="n">
+      <c r="BE2" s="27" t="n">
+        <f aca="false">BB2</f>
         <v>28</v>
       </c>
-      <c r="BC2" s="25"/>
-      <c r="BD2" s="24" t="n">
+      <c r="BF2" s="28"/>
+      <c r="BG2" s="27" t="n">
+        <f aca="false">BE2+BE4</f>
         <v>29</v>
       </c>
-      <c r="BG2" s="24" t="n">
+      <c r="BJ2" s="27" t="n">
+        <f aca="false">BG2</f>
         <v>29</v>
       </c>
-      <c r="BH2" s="25"/>
-      <c r="BI2" s="24" t="n">
+      <c r="BK2" s="28"/>
+      <c r="BL2" s="27" t="n">
+        <f aca="false">BJ2+BJ4</f>
         <v>34</v>
       </c>
-      <c r="BL2" s="24" t="n">
+      <c r="BO2" s="27" t="n">
+        <f aca="false">MAX(BL2,AC14)</f>
         <v>34</v>
       </c>
-      <c r="BM2" s="25"/>
-      <c r="BN2" s="24" t="n">
+      <c r="BP2" s="28"/>
+      <c r="BQ2" s="27" t="n">
+        <f aca="false">BO2+BO4</f>
         <v>35</v>
       </c>
     </row>
@@ -3247,70 +3351,80 @@
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="27" t="n">
+      <c r="F3" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="30" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="28" t="s">
+      <c r="H3" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="30" t="n">
+        <f aca="false">ROUND(G3/(H3*I3),0)</f>
+        <v>1</v>
+      </c>
+      <c r="L3" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="N3" s="28" t="s">
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="Q3" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="S3" s="28" t="s">
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="V3" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="AC3" s="28" t="s">
+      <c r="W3" s="32"/>
+      <c r="X3" s="32"/>
+      <c r="AF3" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="AD3" s="28"/>
-      <c r="AE3" s="28"/>
-      <c r="AH3" s="28" t="s">
+      <c r="AG3" s="32"/>
+      <c r="AH3" s="32"/>
+      <c r="AK3" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="AI3" s="28"/>
-      <c r="AJ3" s="28"/>
-      <c r="AM3" s="28" t="s">
+      <c r="AL3" s="32"/>
+      <c r="AM3" s="32"/>
+      <c r="AP3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="AN3" s="28"/>
-      <c r="AO3" s="28"/>
-      <c r="AR3" s="28" t="s">
+      <c r="AQ3" s="32"/>
+      <c r="AR3" s="32"/>
+      <c r="AU3" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="AS3" s="28"/>
-      <c r="AT3" s="28"/>
-      <c r="AW3" s="28" t="s">
+      <c r="AV3" s="32"/>
+      <c r="AW3" s="32"/>
+      <c r="AZ3" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="AX3" s="28"/>
-      <c r="AY3" s="28"/>
-      <c r="BB3" s="28" t="s">
+      <c r="BA3" s="32"/>
+      <c r="BB3" s="32"/>
+      <c r="BE3" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="BC3" s="28"/>
-      <c r="BD3" s="28"/>
-      <c r="BG3" s="28" t="s">
+      <c r="BF3" s="32"/>
+      <c r="BG3" s="32"/>
+      <c r="BJ3" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="BH3" s="28"/>
-      <c r="BI3" s="28"/>
-      <c r="BL3" s="28" t="s">
+      <c r="BK3" s="32"/>
+      <c r="BL3" s="32"/>
+      <c r="BO3" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="BM3" s="28"/>
-      <c r="BN3" s="28"/>
+      <c r="BP3" s="32"/>
+      <c r="BQ3" s="32"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
@@ -3321,123 +3435,154 @@
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="15"/>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="27" t="n">
+      <c r="G4" s="30" t="n">
         <v>4</v>
       </c>
-      <c r="I4" s="29" t="n">
-        <f aca="false">G2</f>
+      <c r="H4" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="30" t="n">
+        <f aca="false">ROUND(G4/(H4*I4),0)</f>
+        <v>4</v>
+      </c>
+      <c r="L4" s="33" t="n">
+        <f aca="false">J2</f>
         <v>5</v>
       </c>
-      <c r="J4" s="30" t="n">
+      <c r="M4" s="34" t="n">
+        <f aca="false">N5-N2</f>
         <v>0</v>
       </c>
-      <c r="K4" s="29" t="n">
+      <c r="N4" s="33" t="n">
+        <f aca="false">MIN(Q2,Q14)-N2</f>
         <v>0</v>
       </c>
-      <c r="N4" s="29" t="n">
-        <f aca="false">G3</f>
+      <c r="Q4" s="33" t="n">
+        <f aca="false">J3</f>
         <v>1</v>
       </c>
-      <c r="O4" s="30" t="n">
+      <c r="R4" s="34" t="n">
+        <f aca="false">S5-S2</f>
         <v>0</v>
       </c>
-      <c r="P4" s="29" t="n">
+      <c r="S4" s="33" t="n">
+        <f aca="false">MIN(V2,V8)-S2</f>
         <v>0</v>
       </c>
-      <c r="S4" s="29" t="n">
-        <f aca="false">G4</f>
+      <c r="V4" s="33" t="n">
+        <f aca="false">J4</f>
         <v>4</v>
       </c>
-      <c r="T4" s="31" t="n">
+      <c r="W4" s="34" t="n">
+        <f aca="false">X5-X2</f>
         <v>6</v>
       </c>
-      <c r="U4" s="29" t="n">
+      <c r="X4" s="33" t="n">
+        <f aca="false">AF2-X2</f>
         <v>6</v>
       </c>
-      <c r="AC4" s="29" t="n">
-        <f aca="false">G9</f>
+      <c r="AF4" s="33" t="n">
+        <f aca="false">J9</f>
         <v>2</v>
       </c>
-      <c r="AD4" s="30" t="n">
+      <c r="AG4" s="34" t="n">
+        <f aca="false">AH5-AH2</f>
         <v>0</v>
       </c>
-      <c r="AE4" s="29" t="n">
+      <c r="AH4" s="33" t="n">
+        <f aca="false">AK2-AH2</f>
         <v>0</v>
       </c>
-      <c r="AH4" s="29" t="n">
-        <f aca="false">G10</f>
+      <c r="AK4" s="33" t="n">
+        <f aca="false">J10</f>
         <v>2</v>
       </c>
-      <c r="AI4" s="30" t="n">
+      <c r="AL4" s="34" t="n">
+        <f aca="false">AM5-AM2</f>
         <v>0</v>
       </c>
-      <c r="AJ4" s="29" t="n">
+      <c r="AM4" s="33" t="n">
+        <f aca="false">AP2-AM2</f>
         <v>0</v>
       </c>
-      <c r="AM4" s="29" t="n">
-        <f aca="false">G11</f>
+      <c r="AP4" s="33" t="n">
+        <f aca="false">J11</f>
         <v>2</v>
       </c>
-      <c r="AN4" s="30" t="n">
+      <c r="AQ4" s="34" t="n">
+        <f aca="false">AR5-AR2</f>
         <v>0</v>
       </c>
-      <c r="AO4" s="29" t="n">
+      <c r="AR4" s="33" t="n">
+        <f aca="false">AU2-AR2</f>
         <v>0</v>
       </c>
-      <c r="AR4" s="29" t="n">
-        <f aca="false">G13</f>
+      <c r="AU4" s="33" t="n">
+        <f aca="false">J13</f>
         <v>3</v>
       </c>
-      <c r="AS4" s="30" t="n">
+      <c r="AV4" s="34" t="n">
+        <f aca="false">AW5-AW2</f>
         <v>0</v>
       </c>
-      <c r="AT4" s="29" t="n">
+      <c r="AW4" s="33" t="n">
+        <f aca="false">AZ2-AW2</f>
         <v>0</v>
       </c>
-      <c r="AW4" s="29" t="n">
-        <f aca="false">G14</f>
+      <c r="AZ4" s="33" t="n">
+        <f aca="false">J14</f>
         <v>3</v>
       </c>
-      <c r="AX4" s="30" t="n">
+      <c r="BA4" s="34" t="n">
+        <f aca="false">BB5-BB2</f>
         <v>0</v>
       </c>
-      <c r="AY4" s="29" t="n">
+      <c r="BB4" s="33" t="n">
+        <f aca="false">BE2-BB2</f>
         <v>0</v>
       </c>
-      <c r="BB4" s="29" t="n">
-        <f aca="false">G15</f>
+      <c r="BE4" s="33" t="n">
+        <f aca="false">J15</f>
         <v>1</v>
       </c>
-      <c r="BC4" s="30" t="n">
+      <c r="BF4" s="34" t="n">
+        <f aca="false">BG5-BG2</f>
         <v>0</v>
       </c>
-      <c r="BD4" s="29" t="n">
+      <c r="BG4" s="33" t="n">
+        <f aca="false">BJ2-BG2</f>
         <v>0</v>
       </c>
-      <c r="BG4" s="29" t="n">
-        <f aca="false">G16</f>
+      <c r="BJ4" s="33" t="n">
+        <f aca="false">J16</f>
         <v>5</v>
       </c>
-      <c r="BH4" s="30" t="n">
+      <c r="BK4" s="34" t="n">
+        <f aca="false">BL5-BL2</f>
         <v>0</v>
       </c>
-      <c r="BI4" s="29" t="n">
+      <c r="BL4" s="33" t="n">
+        <f aca="false">BO2-BL2</f>
         <v>0</v>
       </c>
-      <c r="BL4" s="29" t="n">
-        <f aca="false">G17</f>
+      <c r="BO4" s="33" t="n">
+        <f aca="false">J17</f>
         <v>1</v>
       </c>
-      <c r="BM4" s="30" t="n">
+      <c r="BP4" s="34" t="n">
+        <f aca="false">BQ5-BQ2</f>
         <v>0</v>
       </c>
-      <c r="BN4" s="29"/>
+      <c r="BQ4" s="33"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
@@ -3448,90 +3593,122 @@
       </c>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="27" t="n">
+      <c r="G5" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="I5" s="24" t="n">
+      <c r="H5" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="30" t="n">
+        <f aca="false">ROUND(G5/(H5*I5),0)</f>
+        <v>3</v>
+      </c>
+      <c r="L5" s="27" t="n">
+        <f aca="false">N5-L4</f>
         <v>0</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="24" t="n">
+      <c r="M5" s="28"/>
+      <c r="N5" s="27" t="n">
+        <f aca="false">MIN(Q5,Q17)</f>
         <v>5</v>
       </c>
-      <c r="N5" s="24" t="n">
+      <c r="Q5" s="27" t="n">
+        <f aca="false">S5-Q4</f>
         <v>5</v>
       </c>
-      <c r="O5" s="25"/>
-      <c r="P5" s="24" t="n">
+      <c r="R5" s="28"/>
+      <c r="S5" s="27" t="n">
+        <f aca="false">MIN(V5,V11)</f>
         <v>6</v>
       </c>
-      <c r="S5" s="24" t="n">
+      <c r="V5" s="27" t="n">
+        <f aca="false">X5-V4</f>
         <v>12</v>
       </c>
-      <c r="T5" s="25"/>
-      <c r="U5" s="24" t="n">
+      <c r="W5" s="28"/>
+      <c r="X5" s="27" t="n">
+        <f aca="false">AF5</f>
         <v>16</v>
       </c>
-      <c r="AC5" s="24" t="n">
+      <c r="AF5" s="27" t="n">
+        <f aca="false">AH5-AF4</f>
         <v>16</v>
       </c>
-      <c r="AD5" s="25"/>
-      <c r="AE5" s="24" t="n">
+      <c r="AG5" s="28"/>
+      <c r="AH5" s="27" t="n">
+        <f aca="false">AK5</f>
         <v>18</v>
       </c>
-      <c r="AH5" s="24" t="n">
+      <c r="AK5" s="27" t="n">
+        <f aca="false">AM5-AK4</f>
         <v>18</v>
       </c>
-      <c r="AI5" s="25"/>
-      <c r="AJ5" s="24" t="n">
+      <c r="AL5" s="28"/>
+      <c r="AM5" s="27" t="n">
+        <f aca="false">AP5</f>
         <v>20</v>
       </c>
-      <c r="AM5" s="24" t="n">
+      <c r="AP5" s="27" t="n">
+        <f aca="false">AR5-AP4</f>
         <v>20</v>
       </c>
-      <c r="AN5" s="25"/>
-      <c r="AO5" s="24" t="n">
+      <c r="AQ5" s="28"/>
+      <c r="AR5" s="27" t="n">
+        <f aca="false">AU5</f>
         <v>22</v>
       </c>
-      <c r="AR5" s="24" t="n">
+      <c r="AU5" s="27" t="n">
+        <f aca="false">AW5-AU4</f>
         <v>22</v>
       </c>
-      <c r="AS5" s="25"/>
-      <c r="AT5" s="24" t="n">
+      <c r="AV5" s="28"/>
+      <c r="AW5" s="27" t="n">
+        <f aca="false">AZ5</f>
         <v>25</v>
       </c>
-      <c r="AW5" s="24" t="n">
+      <c r="AZ5" s="27" t="n">
+        <f aca="false">BB5-AZ4</f>
         <v>25</v>
       </c>
-      <c r="AX5" s="25"/>
-      <c r="AY5" s="24" t="n">
+      <c r="BA5" s="28"/>
+      <c r="BB5" s="27" t="n">
+        <f aca="false">BE5</f>
         <v>28</v>
       </c>
-      <c r="BB5" s="24" t="n">
+      <c r="BE5" s="27" t="n">
+        <f aca="false">BG5-BE4</f>
         <v>28</v>
       </c>
-      <c r="BC5" s="25"/>
-      <c r="BD5" s="24" t="n">
+      <c r="BF5" s="28"/>
+      <c r="BG5" s="27" t="n">
+        <f aca="false">BJ5</f>
         <v>29</v>
       </c>
-      <c r="BG5" s="24" t="n">
+      <c r="BJ5" s="27" t="n">
+        <f aca="false">BL5-BJ4</f>
         <v>29</v>
       </c>
-      <c r="BH5" s="25"/>
-      <c r="BI5" s="24" t="n">
+      <c r="BK5" s="28"/>
+      <c r="BL5" s="27" t="n">
+        <f aca="false">BO5</f>
         <v>34</v>
       </c>
-      <c r="BL5" s="24" t="n">
+      <c r="BO5" s="27" t="n">
+        <f aca="false">BQ5-BO4</f>
         <v>34</v>
       </c>
-      <c r="BM5" s="25"/>
-      <c r="BN5" s="24" t="n">
+      <c r="BP5" s="28"/>
+      <c r="BQ5" s="27" t="n">
+        <f aca="false">BQ2</f>
         <v>35</v>
       </c>
     </row>
@@ -3544,13 +3721,23 @@
       </c>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="F6" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="33" t="n">
+      <c r="G6" s="36" t="n">
+        <v>7</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="30" t="n">
+        <f aca="false">ROUND(G6/(H6*I6),0)</f>
         <v>7</v>
       </c>
     </row>
@@ -3563,13 +3750,23 @@
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="27" t="n">
+      <c r="G7" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="30" t="n">
+        <f aca="false">ROUND(G7/(H7*I7),0)</f>
         <v>1</v>
       </c>
     </row>
@@ -3582,27 +3779,41 @@
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="33" t="n">
+      <c r="F8" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="36" t="n">
         <v>3</v>
       </c>
-      <c r="S8" s="24" t="n">
+      <c r="H8" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="30" t="n">
+        <f aca="false">ROUND(G8/(H8*I8),0)</f>
+        <v>3</v>
+      </c>
+      <c r="V8" s="27" t="n">
+        <f aca="false">S2</f>
         <v>6</v>
       </c>
-      <c r="T8" s="25"/>
-      <c r="U8" s="24" t="n">
+      <c r="W8" s="28"/>
+      <c r="X8" s="27" t="n">
+        <f aca="false">V8+V10</f>
         <v>9</v>
       </c>
-      <c r="X8" s="24" t="n">
+      <c r="AA8" s="27" t="n">
+        <f aca="false">X8</f>
         <v>9</v>
       </c>
-      <c r="Y8" s="25"/>
-      <c r="Z8" s="24" t="n">
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="27" t="n">
+        <f aca="false">AA8+AA10</f>
         <v>16</v>
       </c>
     </row>
@@ -3615,25 +3826,35 @@
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="36" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="33" t="n">
+      <c r="I9" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="30" t="n">
+        <f aca="false">ROUND(G9/(H9*I9),0)</f>
         <v>2</v>
       </c>
-      <c r="S9" s="28" t="s">
+      <c r="V9" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="X9" s="28" t="s">
+      <c r="W9" s="32"/>
+      <c r="X9" s="32"/>
+      <c r="AA9" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
+      <c r="AB9" s="32"/>
+      <c r="AC9" s="32"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
@@ -3644,33 +3865,47 @@
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="33" t="n">
+      <c r="G10" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="S10" s="29" t="n">
-        <f aca="false">G5</f>
+      <c r="H10" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I10" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="30" t="n">
+        <f aca="false">ROUND(G10/(H10*I10),0)</f>
+        <v>2</v>
+      </c>
+      <c r="V10" s="33" t="n">
+        <f aca="false">J5</f>
         <v>3</v>
       </c>
-      <c r="T10" s="30" t="n">
+      <c r="W10" s="34" t="n">
+        <f aca="false">X11-X8</f>
         <v>0</v>
       </c>
-      <c r="U10" s="29" t="n">
+      <c r="X10" s="33" t="n">
+        <f aca="false">AA8-X8</f>
         <v>0</v>
       </c>
-      <c r="X10" s="29" t="n">
-        <f aca="false">G6</f>
+      <c r="AA10" s="33" t="n">
+        <f aca="false">J6</f>
         <v>7</v>
       </c>
-      <c r="Y10" s="30" t="n">
+      <c r="AB10" s="34" t="n">
+        <f aca="false">AC11-AC8</f>
         <v>0</v>
       </c>
-      <c r="Z10" s="29" t="n">
+      <c r="AC10" s="33" t="n">
+        <f aca="false">AF2-AC8</f>
         <v>0</v>
       </c>
     </row>
@@ -3683,27 +3918,41 @@
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="33" t="n">
+      <c r="G11" s="36" t="n">
         <v>2</v>
       </c>
-      <c r="S11" s="24" t="n">
+      <c r="H11" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="30" t="n">
+        <f aca="false">ROUND(G11/(H11*I11),0)</f>
+        <v>2</v>
+      </c>
+      <c r="V11" s="27" t="n">
+        <f aca="false">X11-V10</f>
         <v>6</v>
       </c>
-      <c r="T11" s="25"/>
-      <c r="U11" s="24" t="n">
+      <c r="W11" s="28"/>
+      <c r="X11" s="27" t="n">
+        <f aca="false">AA11</f>
         <v>9</v>
       </c>
-      <c r="X11" s="24" t="n">
+      <c r="AA11" s="27" t="n">
+        <f aca="false">AC11-AA10</f>
         <v>9</v>
       </c>
-      <c r="Y11" s="25"/>
-      <c r="Z11" s="24" t="n">
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="27" t="n">
+        <f aca="false">AF5</f>
         <v>16</v>
       </c>
     </row>
@@ -3712,17 +3961,27 @@
         <v>17</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="33" t="n">
+      <c r="G12" s="36" t="n">
+        <v>10</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="30" t="n">
+        <f aca="false">ROUND(G12/(H12*I12),0)</f>
         <v>10</v>
       </c>
     </row>
@@ -3735,13 +3994,23 @@
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="33" t="n">
+      <c r="G13" s="36" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="30" t="n">
+        <f aca="false">ROUND(G13/(H13*I13),0)</f>
         <v>3</v>
       </c>
     </row>
@@ -3754,34 +4023,50 @@
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="33" t="n">
+      <c r="G14" s="36" t="n">
         <v>3</v>
       </c>
-      <c r="N14" s="24" t="n">
+      <c r="H14" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="30" t="n">
+        <f aca="false">ROUND(G14/(H14*I14),0)</f>
+        <v>3</v>
+      </c>
+      <c r="Q14" s="27" t="n">
+        <f aca="false">N2</f>
         <v>5</v>
       </c>
-      <c r="O14" s="25"/>
-      <c r="P14" s="24" t="n">
+      <c r="R14" s="28"/>
+      <c r="S14" s="27" t="n">
+        <f aca="false">Q14+Q16</f>
         <v>6</v>
       </c>
-      <c r="S14" s="24" t="n">
+      <c r="V14" s="27" t="n">
+        <f aca="false">S14</f>
         <v>6</v>
       </c>
-      <c r="T14" s="25"/>
-      <c r="U14" s="24" t="n">
+      <c r="W14" s="28"/>
+      <c r="X14" s="27" t="n">
+        <f aca="false">V14+V16</f>
         <v>9</v>
       </c>
-      <c r="X14" s="24" t="n">
+      <c r="AA14" s="27" t="n">
+        <f aca="false">X14</f>
         <v>9</v>
       </c>
-      <c r="Y14" s="25"/>
-      <c r="Z14" s="24" t="n">
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="27" t="n">
+        <f aca="false">AA14+AA16</f>
         <v>19</v>
       </c>
     </row>
@@ -3794,30 +4079,40 @@
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="33" t="n">
+      <c r="G15" s="36" t="n">
         <v>1</v>
       </c>
-      <c r="N15" s="28" t="s">
+      <c r="H15" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="30" t="n">
+        <f aca="false">ROUND(G15/(H15*I15),0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q15" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="O15" s="28"/>
-      <c r="P15" s="28"/>
-      <c r="S15" s="28" t="s">
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="V15" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="X15" s="28" t="s">
+      <c r="W15" s="32"/>
+      <c r="X15" s="32"/>
+      <c r="AA15" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="Y15" s="28"/>
-      <c r="Z15" s="28"/>
+      <c r="AB15" s="32"/>
+      <c r="AC15" s="32"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="s">
@@ -3828,43 +4123,59 @@
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="G16" s="33" t="n">
+      <c r="G16" s="36" t="n">
         <v>5</v>
       </c>
-      <c r="N16" s="29" t="n">
-        <f aca="false">G7</f>
+      <c r="H16" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="O16" s="31" t="n">
+      <c r="J16" s="30" t="n">
+        <f aca="false">ROUND(G16/(H16*I16),0)</f>
+        <v>5</v>
+      </c>
+      <c r="Q16" s="33" t="n">
+        <f aca="false">J7</f>
+        <v>1</v>
+      </c>
+      <c r="R16" s="34" t="n">
+        <f aca="false">S17-S14</f>
         <v>7</v>
       </c>
-      <c r="P16" s="29" t="n">
+      <c r="S16" s="33" t="n">
+        <f aca="false">V14-S14</f>
         <v>0</v>
       </c>
-      <c r="S16" s="29" t="n">
-        <f aca="false">G8</f>
+      <c r="V16" s="33" t="n">
+        <f aca="false">J8</f>
         <v>3</v>
       </c>
-      <c r="T16" s="31" t="n">
+      <c r="W16" s="34" t="n">
+        <f aca="false">X17-X14</f>
         <v>7</v>
       </c>
-      <c r="U16" s="29" t="n">
+      <c r="X16" s="33" t="n">
+        <f aca="false">MIN(AA14,AF2)-X14</f>
         <v>0</v>
       </c>
-      <c r="X16" s="29" t="n">
-        <f aca="false">G12</f>
+      <c r="AA16" s="33" t="n">
+        <f aca="false">J12</f>
         <v>10</v>
       </c>
-      <c r="Y16" s="31" t="n">
+      <c r="AB16" s="34" t="n">
+        <f aca="false">AC17-AC14</f>
         <v>15</v>
       </c>
-      <c r="Z16" s="29" t="n">
+      <c r="AC16" s="33" t="n">
+        <f aca="false">BO2-AC14</f>
         <v>15</v>
       </c>
     </row>
@@ -3877,32 +4188,48 @@
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="35"/>
-      <c r="G17" s="36" t="n">
+      <c r="E17" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="N17" s="24" t="n">
+      <c r="H17" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="40" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="39" t="n">
+        <f aca="false">ROUND(G17/(H17*I17),0)</f>
+        <v>1</v>
+      </c>
+      <c r="Q17" s="27" t="n">
+        <f aca="false">S17-Q16</f>
         <v>12</v>
       </c>
-      <c r="O17" s="25"/>
-      <c r="P17" s="24" t="n">
+      <c r="R17" s="28"/>
+      <c r="S17" s="27" t="n">
+        <f aca="false">V17</f>
         <v>13</v>
       </c>
-      <c r="S17" s="24" t="n">
+      <c r="V17" s="27" t="n">
+        <f aca="false">X17-V16</f>
         <v>13</v>
       </c>
-      <c r="T17" s="25"/>
-      <c r="U17" s="24" t="n">
+      <c r="W17" s="28"/>
+      <c r="X17" s="27" t="n">
+        <f aca="false">MIN(AA17,AF5)</f>
         <v>16</v>
       </c>
-      <c r="X17" s="24" t="n">
+      <c r="AA17" s="27" t="n">
+        <f aca="false">AC17-AA16</f>
         <v>24</v>
       </c>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="24" t="n">
+      <c r="AB17" s="28"/>
+      <c r="AC17" s="27" t="n">
+        <f aca="false">BO5</f>
         <v>34</v>
       </c>
     </row>
@@ -3911,37 +4238,42 @@
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="AC3:AE3"/>
-    <mergeCell ref="AH3:AJ3"/>
-    <mergeCell ref="AM3:AO3"/>
-    <mergeCell ref="AR3:AT3"/>
-    <mergeCell ref="AW3:AY3"/>
-    <mergeCell ref="BB3:BD3"/>
-    <mergeCell ref="BG3:BI3"/>
-    <mergeCell ref="BL3:BN3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AP3:AR3"/>
+    <mergeCell ref="AU3:AW3"/>
+    <mergeCell ref="AZ3:BB3"/>
+    <mergeCell ref="BE3:BG3"/>
+    <mergeCell ref="BJ3:BL3"/>
+    <mergeCell ref="BO3:BQ3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="X9:Z9"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="AA9:AC9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="X15:Z15"/>
+    <mergeCell ref="Q15:S15"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="AA15:AC15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
   </mergeCells>
+  <conditionalFormatting sqref="M4 R4 R16 W4 W10 W16 AB10 AB16 AG4 AL4 AQ4 AV4 BA4 BF4 BK4 BP4">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Formel für Ressourcenplanung (Dauer).
</commit_message>
<xml_diff>
--- a/Online_Shop.Projekt.xlsx
+++ b/Online_Shop.Projekt.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="59">
   <si>
     <t xml:space="preserve">Beispiel: Funktionsorientierter Projektstrukturplan</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kapazität</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dauer</t>
   </si>
   <si>
     <t xml:space="preserve">1.1.1, 1.2.2</t>
@@ -368,7 +371,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -531,6 +534,10 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -639,7 +646,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8118360" y="325080"/>
+          <a:off x="8127000" y="325080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -663,13 +670,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>883800</xdr:colOff>
+      <xdr:colOff>884160</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>900360</xdr:colOff>
+      <xdr:colOff>900720</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
@@ -680,8 +687,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5399280" y="479520"/>
-          <a:ext cx="5438160" cy="0"/>
+          <a:off x="5404320" y="479520"/>
+          <a:ext cx="5445720" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -721,7 +728,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5418720" y="488160"/>
+          <a:off x="5424840" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -762,7 +769,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5419800" y="488160"/>
+          <a:off x="5425920" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -803,7 +810,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8130600" y="488160"/>
+          <a:off x="8140680" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -844,7 +851,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10841040" y="488160"/>
+          <a:off x="10854720" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -885,7 +892,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5419800" y="1122120"/>
+          <a:off x="5425920" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -926,7 +933,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5419800" y="1609560"/>
+          <a:off x="5425920" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -967,7 +974,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5419800" y="2097720"/>
+          <a:off x="5425920" y="2097720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1008,7 +1015,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5419800" y="2584800"/>
+          <a:off x="5425920" y="2584800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1049,7 +1056,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8130600" y="1122120"/>
+          <a:off x="8140680" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1090,7 +1097,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8130600" y="1609560"/>
+          <a:off x="8140680" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1131,7 +1138,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8130600" y="2097720"/>
+          <a:off x="8140680" y="2097720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1172,7 +1179,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8130600" y="2584800"/>
+          <a:off x="8140680" y="2584800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1213,7 +1220,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8130600" y="3072240"/>
+          <a:off x="8140680" y="3072240"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1254,7 +1261,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8130600" y="3560400"/>
+          <a:off x="8140680" y="3560400"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1295,7 +1302,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8130600" y="4047480"/>
+          <a:off x="8140680" y="4047480"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1336,7 +1343,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8130600" y="4534920"/>
+          <a:off x="8140680" y="4534920"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1377,7 +1384,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8130600" y="5023080"/>
+          <a:off x="8140680" y="5023080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1418,7 +1425,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10841400" y="2097360"/>
+          <a:off x="10855080" y="2097360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1459,7 +1466,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10841400" y="1609560"/>
+          <a:off x="10855080" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1500,7 +1507,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10841400" y="1121760"/>
+          <a:off x="10855080" y="1121760"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1529,15 +1536,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>7560</xdr:colOff>
+      <xdr:colOff>8280</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>2520</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1546,7 +1553,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7113240" y="475920"/>
+          <a:off x="7119000" y="476280"/>
           <a:ext cx="535320" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1573,13 +1580,13 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>264960</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>265320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1588,7 +1595,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8453160" y="482040"/>
+          <a:off x="8458200" y="482400"/>
           <a:ext cx="541440" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1613,15 +1620,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>253440</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>271080</xdr:colOff>
+      <xdr:rowOff>13680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1630,7 +1637,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7359120" y="500040"/>
+          <a:off x="7364520" y="500760"/>
           <a:ext cx="18000" cy="1950840"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1655,15 +1662,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>7200</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>259560</xdr:colOff>
+      <xdr:colOff>259920</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1672,7 +1679,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7383600" y="2432880"/>
+          <a:off x="7389000" y="2433240"/>
           <a:ext cx="252360" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1697,15 +1704,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>241200</xdr:colOff>
+      <xdr:colOff>241920</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>156960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1714,50 +1721,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9812160" y="475920"/>
+          <a:off x="9817920" y="476280"/>
           <a:ext cx="1863000" cy="5400"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>255960</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>270000</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="11419200" y="491040"/>
-          <a:ext cx="284760" cy="2160"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1783,13 +1748,55 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>264600</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>264960</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
+      <xdr:rowOff>163440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8457840" y="2433960"/>
+          <a:ext cx="541440" cy="5040"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>264600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>158400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>259200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1797,9 +1804,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="8452800" y="2433600"/>
-          <a:ext cx="541440" cy="5040"/>
+        <a:xfrm flipV="1">
+          <a:off x="9810360" y="2433960"/>
+          <a:ext cx="535680" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1822,26 +1829,110 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>256320</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>155520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>256320</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8719920" y="480240"/>
+          <a:ext cx="0" cy="982440"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>250200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>254880</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8713440" y="1452600"/>
+          <a:ext cx="275400" cy="3960"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>264240</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>258840</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9804960" y="2433600"/>
-          <a:ext cx="535680" cy="5040"/>
+      <xdr:colOff>256680</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>155520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>11520</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>162720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9802080" y="1455840"/>
+          <a:ext cx="566280" cy="7200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1864,142 +1955,58 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>255960</xdr:colOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>261000</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>155160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>255960</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>162360</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8714520" y="480240"/>
-          <a:ext cx="0" cy="982440"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>254160</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="8707680" y="1452240"/>
-          <a:ext cx="275400" cy="3960"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>255960</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>10800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9796320" y="1455840"/>
-          <a:ext cx="566280" cy="7200"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>260640</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>9360</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>155160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>155160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12511800" y="480240"/>
+          <a:ext cx="559800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>261360</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>138600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>271440</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2007,9 +2014,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12506400" y="480240"/>
-          <a:ext cx="559800" cy="0"/>
+        <a:xfrm flipH="1">
+          <a:off x="10077480" y="1926720"/>
+          <a:ext cx="10080" cy="505440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2035,13 +2042,13 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>261000</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>271080</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>153000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>253800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2049,93 +2056,51 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10077120" y="1940760"/>
+          <a:ext cx="1345680" cy="4680"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>259920</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>144000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>261000</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>23040</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10072080" y="1926720"/>
-          <a:ext cx="10080" cy="505440"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>260640</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>253440</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="10071360" y="1940400"/>
-          <a:ext cx="1345320" cy="4680"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>259560</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>271080</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>22320</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="11423160" y="593280"/>
-          <a:ext cx="11520" cy="1379520"/>
+          <a:off x="11428560" y="468720"/>
+          <a:ext cx="1080" cy="1504440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2171,13 +2136,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name=""/>
+        <xdr:cNvPr id="36" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11164320" y="1463040"/>
-          <a:ext cx="278280" cy="0"/>
+          <a:off x="11169720" y="1463040"/>
+          <a:ext cx="277920" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2213,13 +2178,13 @@
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name=""/>
+        <xdr:cNvPr id="37" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13877640" y="478440"/>
-          <a:ext cx="559440" cy="0"/>
+          <a:off x="13882680" y="478440"/>
+          <a:ext cx="559800" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2243,24 +2208,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>269280</xdr:colOff>
+      <xdr:colOff>270000</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>13680</xdr:colOff>
+      <xdr:colOff>14400</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name=""/>
+        <xdr:cNvPr id="38" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15219720" y="478080"/>
+          <a:off x="15225480" y="478080"/>
           <a:ext cx="556200" cy="3600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2287,22 +2252,22 @@
       <xdr:col>49</xdr:col>
       <xdr:colOff>18720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>6840</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name=""/>
+      <xdr:rowOff>163080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="16592760" y="482040"/>
+          <a:off x="16597800" y="482400"/>
           <a:ext cx="529200" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2329,13 +2294,55 @@
       <xdr:col>53</xdr:col>
       <xdr:colOff>249480</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
       <xdr:colOff>19080</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>154080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17910720" y="477720"/>
+          <a:ext cx="581040" cy="1080"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>249840</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>154080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>60</xdr:col>
+      <xdr:colOff>260280</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2343,50 +2350,8 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17904960" y="477360"/>
-          <a:ext cx="581400" cy="1080"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>58</xdr:col>
-      <xdr:colOff>249480</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>60</xdr:col>
-      <xdr:colOff>259920</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="19257840" y="478440"/>
+          <a:off x="19263240" y="478800"/>
           <a:ext cx="551160" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2413,13 +2378,55 @@
       <xdr:col>63</xdr:col>
       <xdr:colOff>269280</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>65</xdr:col>
       <xdr:colOff>269640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>163080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="20635560" y="478800"/>
+          <a:ext cx="541440" cy="9000"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>260280</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>266400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>163440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2427,9 +2434,51 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20896560" y="488520"/>
+          <a:ext cx="6120" cy="1950480"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>7200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>157680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>259200</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="20630160" y="478440"/>
-          <a:ext cx="541080" cy="9000"/>
+          <a:off x="8470800" y="482400"/>
+          <a:ext cx="252000" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2452,151 +2501,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>64</xdr:col>
-      <xdr:colOff>259560</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>64</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>265680</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>163080</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name=""/>
+      <xdr:rowOff>158040</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>251280</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="45" name=""/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20890800" y="488160"/>
-          <a:ext cx="6120" cy="1950480"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>258840</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="45" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8465400" y="482040"/>
-          <a:ext cx="252000" cy="6120"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>51480</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>215280</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>3240</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="11429640" y="488160"/>
-          <a:ext cx="4680" cy="975240"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>64</xdr:col>
-      <xdr:colOff>250560</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11157840" y="2432520"/>
+          <a:off x="11163600" y="2433240"/>
           <a:ext cx="9723960" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2629,10 +2552,10 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="G:I D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.77"/>
   </cols>
@@ -3173,13 +3096,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BQ17"/>
+  <dimension ref="A1:BQ18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="G:I"/>
+      <selection pane="topLeft" activeCell="AE6" activeCellId="0" sqref="AE6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.12"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.52"/>
@@ -3214,7 +3137,7 @@
         <v>50</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3228,13 +3151,13 @@
       <c r="D2" s="12"/>
       <c r="E2" s="23"/>
       <c r="F2" s="24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G2" s="25" t="n">
         <v>5</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I2" s="26" t="n">
         <v>1</v>
@@ -3355,13 +3278,13 @@
         <v>16</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G3" s="30" t="n">
         <v>1</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I3" s="31" t="n">
         <v>1</v>
@@ -3445,7 +3368,7 @@
         <v>4</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I4" s="31" t="n">
         <v>1</v>
@@ -3603,7 +3526,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I5" s="31" t="n">
         <v>1</v>
@@ -3731,7 +3654,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I6" s="31" t="n">
         <v>1</v>
@@ -3760,7 +3683,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I7" s="31" t="n">
         <v>1</v>
@@ -3783,13 +3706,13 @@
         <v>22</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G8" s="36" t="n">
         <v>3</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I8" s="31" t="n">
         <v>1</v>
@@ -3827,7 +3750,7 @@
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F9" s="35" t="s">
         <v>33</v>
@@ -3836,7 +3759,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I9" s="31" t="n">
         <v>1</v>
@@ -3875,7 +3798,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I10" s="31" t="n">
         <v>1</v>
@@ -3928,7 +3851,7 @@
         <v>2</v>
       </c>
       <c r="H11" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I11" s="31" t="n">
         <v>1</v>
@@ -3961,7 +3884,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -3975,7 +3898,7 @@
         <v>10</v>
       </c>
       <c r="H12" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I12" s="31" t="n">
         <v>1</v>
@@ -4004,7 +3927,7 @@
         <v>3</v>
       </c>
       <c r="H13" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I13" s="31" t="n">
         <v>1</v>
@@ -4033,7 +3956,7 @@
         <v>3</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I14" s="31" t="n">
         <v>1</v>
@@ -4089,7 +4012,7 @@
         <v>1</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I15" s="31" t="n">
         <v>1</v>
@@ -4133,7 +4056,7 @@
         <v>5</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I16" s="31" t="n">
         <v>1</v>
@@ -4189,14 +4112,14 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F17" s="38"/>
       <c r="G17" s="39" t="n">
         <v>1</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I17" s="40" t="n">
         <v>1</v>
@@ -4233,8 +4156,13 @@
         <v>34</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+    </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="34">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:D3"/>
@@ -4268,6 +4196,7 @@
     <mergeCell ref="AA15:AC15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="G18:I18"/>
   </mergeCells>
   <conditionalFormatting sqref="M4 R4 R16 W4 W10 W16 AB10 AB16 AG4 AL4 AQ4 AV4 BA4 BF4 BK4 BP4">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">

</xml_diff>

<commit_message>
Netzplan Projekt OnlineShop FIAE B
</commit_message>
<xml_diff>
--- a/Online_Shop.Projekt.xlsx
+++ b/Online_Shop.Projekt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PSP" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="68">
   <si>
     <t xml:space="preserve">Beispiel: Funktionsorientierter Projektstrukturplan</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t xml:space="preserve">1.1.2, 1.1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">1.2.4, 1.3.1</t>
@@ -614,10 +611,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -660,6 +653,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -824,7 +821,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8162640" y="325080"/>
+          <a:off x="8171640" y="325080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -848,13 +845,13 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>884880</xdr:colOff>
+      <xdr:colOff>885240</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>901440</xdr:colOff>
+      <xdr:colOff>901800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
@@ -865,8 +862,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5425560" y="479520"/>
-          <a:ext cx="5476320" cy="0"/>
+          <a:off x="5430600" y="479520"/>
+          <a:ext cx="5483880" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -906,7 +903,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5447520" y="488160"/>
+          <a:off x="5452560" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -947,7 +944,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5451480" y="488160"/>
+          <a:off x="5457600" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -988,7 +985,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181360" y="488160"/>
+          <a:off x="8191440" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1029,7 +1026,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10910880" y="488160"/>
+          <a:off x="10924560" y="488160"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1070,7 +1067,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5451480" y="1122120"/>
+          <a:off x="5457600" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1111,7 +1108,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5451480" y="1609560"/>
+          <a:off x="5457600" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1152,7 +1149,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5451480" y="2097720"/>
+          <a:off x="5457600" y="2097720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1193,7 +1190,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5451480" y="2584800"/>
+          <a:off x="5457600" y="2584800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1234,7 +1231,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181360" y="1122120"/>
+          <a:off x="8191440" y="1122120"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1275,7 +1272,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181360" y="1609560"/>
+          <a:off x="8191440" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1316,7 +1313,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181360" y="2097720"/>
+          <a:off x="8191440" y="2097720"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1357,7 +1354,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181360" y="2584800"/>
+          <a:off x="8191440" y="2584800"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1398,7 +1395,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181360" y="3072240"/>
+          <a:off x="8191440" y="3072240"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1439,7 +1436,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181360" y="3560400"/>
+          <a:off x="8191440" y="3560400"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1480,7 +1477,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181360" y="4047480"/>
+          <a:off x="8191440" y="4047480"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1521,7 +1518,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181360" y="4534920"/>
+          <a:off x="8191440" y="4534920"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1562,7 +1559,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8181360" y="5023080"/>
+          <a:off x="8191440" y="5023080"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1603,7 +1600,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10911240" y="2097360"/>
+          <a:off x="10924920" y="2097360"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1644,7 +1641,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10911240" y="1609560"/>
+          <a:off x="10924920" y="1609560"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1685,7 +1682,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10911240" y="1121760"/>
+          <a:off x="10924920" y="1121760"/>
           <a:ext cx="0" cy="170640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1716,13 +1713,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>9720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>4320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1731,7 +1728,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="9579600" y="477720"/>
+          <a:off x="9582120" y="478080"/>
           <a:ext cx="535680" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1756,15 +1753,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>266760</xdr:colOff>
+      <xdr:colOff>267120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1773,7 +1770,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10918440" y="483840"/>
+          <a:off x="10921320" y="484200"/>
           <a:ext cx="541080" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1798,15 +1795,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>253800</xdr:colOff>
+      <xdr:colOff>254160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>16920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>1440</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>16560</xdr:rowOff>
+      <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1815,8 +1812,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9823680" y="503640"/>
-          <a:ext cx="18000" cy="1950840"/>
+          <a:off x="9826200" y="504000"/>
+          <a:ext cx="18360" cy="1950840"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1840,13 +1837,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>10440</xdr:colOff>
+      <xdr:colOff>10800</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>159120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>262800</xdr:colOff>
+      <xdr:colOff>263160</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>159120</xdr:rowOff>
     </xdr:to>
@@ -1857,7 +1854,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9850320" y="2434680"/>
+          <a:off x="9853560" y="2434680"/>
           <a:ext cx="252360" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1882,15 +1879,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>3960</xdr:colOff>
+      <xdr:colOff>4320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>153000</xdr:rowOff>
+      <xdr:rowOff>153360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>243720</xdr:colOff>
+      <xdr:colOff>244080</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
+      <xdr:rowOff>158760</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1899,7 +1896,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12278520" y="477720"/>
+          <a:off x="12281400" y="478080"/>
           <a:ext cx="1863000" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1924,13 +1921,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>266400</xdr:colOff>
+      <xdr:colOff>266760</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>266400</xdr:colOff>
+      <xdr:colOff>266760</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>2160</xdr:rowOff>
     </xdr:to>
@@ -1941,7 +1938,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10918080" y="2435400"/>
+          <a:off x="10920960" y="2435400"/>
           <a:ext cx="541080" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1983,7 +1980,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="12270240" y="2435400"/>
+          <a:off x="12272760" y="2435400"/>
           <a:ext cx="535680" cy="5040"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2010,13 +2007,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>256680</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>156960</xdr:rowOff>
+      <xdr:rowOff>157320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>256680</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1440</xdr:rowOff>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2025,7 +2022,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11179080" y="481680"/>
+          <a:off x="11181600" y="482040"/>
           <a:ext cx="0" cy="982440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2050,15 +2047,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>252000</xdr:colOff>
+      <xdr:colOff>252360</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>154080</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>256680</xdr:colOff>
+      <xdr:colOff>257040</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>158040</xdr:rowOff>
+      <xdr:rowOff>158400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2067,7 +2064,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="11174040" y="1454040"/>
+          <a:off x="11176920" y="1454400"/>
           <a:ext cx="275400" cy="3960"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2109,7 +2106,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12262320" y="1455840"/>
+          <a:off x="12264840" y="1455840"/>
           <a:ext cx="565920" cy="7200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2151,50 +2148,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14970600" y="480240"/>
+          <a:off x="14973120" y="480240"/>
           <a:ext cx="560160" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="36000">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>262800</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>2520</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name=""/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="12537360" y="1926720"/>
-          <a:ext cx="10440" cy="505440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2220,13 +2175,55 @@
       <xdr:col>24</xdr:col>
       <xdr:colOff>263160</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>2880</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12540240" y="1926720"/>
+          <a:ext cx="10440" cy="505440"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>263520</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>255960</xdr:colOff>
+      <xdr:colOff>256320</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2235,7 +2232,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="12537720" y="1942200"/>
+          <a:off x="12540600" y="1942560"/>
           <a:ext cx="1345320" cy="4680"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2260,15 +2257,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>262080</xdr:colOff>
+      <xdr:colOff>262440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>145440</xdr:rowOff>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>263160</xdr:colOff>
+      <xdr:colOff>263520</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2277,7 +2274,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="13889160" y="470160"/>
+          <a:off x="13892040" y="470520"/>
           <a:ext cx="1080" cy="1504440"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2319,7 +2316,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13628880" y="1463040"/>
+          <a:off x="13631400" y="1463040"/>
           <a:ext cx="278280" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2361,8 +2358,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16342560" y="478440"/>
-          <a:ext cx="559800" cy="0"/>
+          <a:off x="16345440" y="478440"/>
+          <a:ext cx="559440" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2386,13 +2383,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>44</xdr:col>
-      <xdr:colOff>1800</xdr:colOff>
+      <xdr:colOff>2160</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>153000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>17280</xdr:colOff>
+      <xdr:colOff>17640</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
@@ -2403,7 +2400,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17686800" y="478080"/>
+          <a:off x="17689680" y="478080"/>
           <a:ext cx="556200" cy="3600"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2430,13 +2427,13 @@
       <xdr:col>49</xdr:col>
       <xdr:colOff>20520</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>8640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2445,8 +2442,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="19058040" y="483840"/>
-          <a:ext cx="528840" cy="5400"/>
+          <a:off x="19060920" y="484200"/>
+          <a:ext cx="529200" cy="5400"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -2472,13 +2469,13 @@
       <xdr:col>53</xdr:col>
       <xdr:colOff>250200</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>56</xdr:col>
       <xdr:colOff>19440</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2487,7 +2484,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20369880" y="479160"/>
+          <a:off x="20372400" y="479520"/>
           <a:ext cx="581040" cy="1080"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2514,13 +2511,13 @@
       <xdr:col>58</xdr:col>
       <xdr:colOff>250920</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
       <xdr:colOff>261360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2529,7 +2526,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="21723120" y="480240"/>
+          <a:off x="21725640" y="480600"/>
           <a:ext cx="551520" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2554,15 +2551,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>155520</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>65</xdr:col>
-      <xdr:colOff>271080</xdr:colOff>
+      <xdr:colOff>271440</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2160</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2571,7 +2568,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="23095440" y="480240"/>
+          <a:off x="23098320" y="480600"/>
           <a:ext cx="541080" cy="9000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2596,13 +2593,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>262080</xdr:colOff>
+      <xdr:colOff>262440</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>2520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>268200</xdr:colOff>
+      <xdr:colOff>268560</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>2160</xdr:rowOff>
     </xdr:to>
@@ -2613,7 +2610,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="23357160" y="489960"/>
+          <a:off x="23360040" y="489960"/>
           <a:ext cx="6120" cy="1950480"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2640,13 +2637,13 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>7560</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>159120</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>259560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>3240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2655,7 +2652,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10929960" y="483840"/>
+          <a:off x="10932480" y="484200"/>
           <a:ext cx="252000" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2680,15 +2677,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
+      <xdr:colOff>267840</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>160920</xdr:rowOff>
+      <xdr:rowOff>161280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>64</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>253440</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2697,7 +2694,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13624200" y="2436120"/>
+          <a:off x="13627080" y="2436480"/>
           <a:ext cx="9723960" cy="6120"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -2733,9 +2730,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>135000</xdr:colOff>
+      <xdr:colOff>134640</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>154800</xdr:rowOff>
+      <xdr:rowOff>154440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2744,8 +2741,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11841480" y="1647720"/>
-          <a:ext cx="126720" cy="155880"/>
+          <a:off x="11850120" y="1647720"/>
+          <a:ext cx="126360" cy="155520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2800,9 +2797,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>132120</xdr:colOff>
+      <xdr:colOff>131760</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>156240</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2811,8 +2808,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13865400" y="2462040"/>
-          <a:ext cx="126720" cy="155880"/>
+          <a:off x="13874400" y="2462040"/>
+          <a:ext cx="126360" cy="155520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2867,9 +2864,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>53</xdr:col>
-      <xdr:colOff>129600</xdr:colOff>
+      <xdr:colOff>129240</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2878,8 +2875,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17156520" y="2949480"/>
-          <a:ext cx="126720" cy="155880"/>
+          <a:off x="17165520" y="2949480"/>
+          <a:ext cx="126360" cy="155520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2939,7 +2936,7 @@
       <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.77"/>
   </cols>
@@ -3482,11 +3479,11 @@
   </sheetPr>
   <dimension ref="A1:BQ18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q15" activeCellId="0" sqref="Q15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="16.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.52"/>
@@ -3578,75 +3575,75 @@
       </c>
       <c r="AF2" s="27" t="n">
         <f aca="false">MAX(X2,AC8,X14)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AG2" s="28"/>
       <c r="AH2" s="27" t="n">
         <f aca="false">AF2+AF4</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AK2" s="27" t="n">
         <f aca="false">AH2</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AL2" s="28"/>
       <c r="AM2" s="27" t="n">
         <f aca="false">AK2+AK4</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AP2" s="27" t="n">
         <f aca="false">AM2</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AQ2" s="28"/>
       <c r="AR2" s="27" t="n">
         <f aca="false">AP2+AP4</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AU2" s="27" t="n">
         <f aca="false">AR2</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AV2" s="28"/>
       <c r="AW2" s="27" t="n">
         <f aca="false">AU2+AU4</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AZ2" s="27" t="n">
         <f aca="false">AW2</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="BA2" s="28"/>
       <c r="BB2" s="27" t="n">
         <f aca="false">AZ2+AZ4</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="BE2" s="27" t="n">
         <f aca="false">BB2</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="BF2" s="28"/>
       <c r="BG2" s="27" t="n">
         <f aca="false">BE2+BE4</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="BJ2" s="27" t="n">
         <f aca="false">BG2</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="BK2" s="28"/>
       <c r="BL2" s="27" t="n">
         <f aca="false">BJ2+BJ4</f>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BO2" s="27" t="n">
         <f aca="false">MAX(BL2,AC14)</f>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BP2" s="28"/>
       <c r="BQ2" s="27" t="n">
         <f aca="false">BO2+BO4</f>
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3791,11 +3788,11 @@
       </c>
       <c r="W4" s="34" t="n">
         <f aca="false">X5-X2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="X4" s="33" t="n">
         <f aca="false">AF2-X2</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AF4" s="33" t="n">
         <f aca="false">J9</f>
@@ -3871,7 +3868,7 @@
       </c>
       <c r="BJ4" s="33" t="n">
         <f aca="false">J16</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="BK4" s="34" t="n">
         <f aca="false">BL5-BL2</f>
@@ -3939,84 +3936,84 @@
       </c>
       <c r="V5" s="27" t="n">
         <f aca="false">X5-V4</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="W5" s="28"/>
       <c r="X5" s="27" t="n">
         <f aca="false">AF5</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AF5" s="27" t="n">
         <f aca="false">AH5-AF4</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AG5" s="28"/>
       <c r="AH5" s="27" t="n">
         <f aca="false">AK5</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AK5" s="27" t="n">
         <f aca="false">AM5-AK4</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AL5" s="28"/>
       <c r="AM5" s="27" t="n">
         <f aca="false">AP5</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AP5" s="27" t="n">
         <f aca="false">AR5-AP4</f>
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="AQ5" s="28"/>
       <c r="AR5" s="27" t="n">
         <f aca="false">AU5</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AU5" s="27" t="n">
         <f aca="false">AW5-AU4</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AV5" s="28"/>
       <c r="AW5" s="27" t="n">
         <f aca="false">AZ5</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="AZ5" s="27" t="n">
         <f aca="false">BB5-AZ4</f>
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="BA5" s="28"/>
       <c r="BB5" s="27" t="n">
         <f aca="false">BE5</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="BE5" s="27" t="n">
         <f aca="false">BG5-BE4</f>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="BF5" s="28"/>
       <c r="BG5" s="27" t="n">
         <f aca="false">BJ5</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="BJ5" s="27" t="n">
         <f aca="false">BL5-BJ4</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="BK5" s="28"/>
       <c r="BL5" s="27" t="n">
         <f aca="false">BO5</f>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BO5" s="27" t="n">
         <f aca="false">BQ5-BO4</f>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="BP5" s="28"/>
       <c r="BQ5" s="27" t="n">
         <f aca="false">BQ2</f>
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4038,15 +4035,14 @@
         <v>7</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I6" s="31" t="n">
-        <f aca="false">(100%+(100%-I12))/2</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J6" s="30" t="n">
         <f aca="false">ROUND(G6/(H6*I6),0)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4091,7 +4087,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="36" t="n">
         <v>3</v>
@@ -4122,7 +4118,7 @@
       <c r="AB8" s="28"/>
       <c r="AC8" s="27" t="n">
         <f aca="false">AA8+AA10</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4135,7 +4131,7 @@
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="35" t="s">
         <v>35</v>
@@ -4206,7 +4202,7 @@
       </c>
       <c r="AA10" s="33" t="n">
         <f aca="false">J6</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AB10" s="34" t="n">
         <f aca="false">AC11-AC8</f>
@@ -4261,7 +4257,7 @@
       <c r="AB11" s="28"/>
       <c r="AC11" s="27" t="n">
         <f aca="false">AF5</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4269,7 +4265,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
@@ -4286,11 +4282,11 @@
         <v>53</v>
       </c>
       <c r="I12" s="31" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J12" s="30" t="n">
         <f aca="false">ROUND(G12/(H12*I12),0)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4375,7 +4371,7 @@
       <c r="AB14" s="28"/>
       <c r="AC14" s="27" t="n">
         <f aca="false">AA14+AA16</f>
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4441,15 +4437,14 @@
         <v>5</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I16" s="31" t="n">
-        <f aca="false">(100%+(100%-$I$12))/2</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J16" s="30" t="n">
         <f aca="false">ROUND(G16/(H16*I16),0)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q16" s="33" t="n">
         <f aca="false">J7</f>
@@ -4457,7 +4452,7 @@
       </c>
       <c r="R16" s="34" t="n">
         <f aca="false">S17-S14</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="S16" s="33" t="n">
         <f aca="false">V14-S14</f>
@@ -4469,7 +4464,7 @@
       </c>
       <c r="W16" s="34" t="n">
         <f aca="false">X17-X14</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="X16" s="33" t="n">
         <f aca="false">MIN(AA14,AF2)-X14</f>
@@ -4477,15 +4472,15 @@
       </c>
       <c r="AA16" s="33" t="n">
         <f aca="false">J12</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AB16" s="34" t="n">
         <f aca="false">AC17-AC14</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="AC16" s="33" t="n">
         <f aca="false">BO2-AC14</f>
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4498,7 +4493,7 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" s="38"/>
       <c r="G17" s="39" t="n">
@@ -4507,7 +4502,7 @@
       <c r="H17" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="40" t="n">
+      <c r="I17" s="31" t="n">
         <v>1</v>
       </c>
       <c r="J17" s="39" t="n">
@@ -4516,30 +4511,30 @@
       </c>
       <c r="Q17" s="27" t="n">
         <f aca="false">S17-Q16</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="R17" s="28"/>
       <c r="S17" s="27" t="n">
         <f aca="false">V17</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="V17" s="27" t="n">
         <f aca="false">X17-V16</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="W17" s="28"/>
       <c r="X17" s="27" t="n">
         <f aca="false">MIN(AA17,AF5)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="AA17" s="27" t="n">
         <f aca="false">AC17-AA16</f>
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="AB17" s="28"/>
       <c r="AC17" s="27" t="n">
         <f aca="false">BO5</f>
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4607,13 +4602,13 @@
   </sheetPr>
   <dimension ref="A1:BN20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="11" ySplit="0" topLeftCell="AU1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="BB14" activeCellId="0" sqref="BB14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="2"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="1" max="5" min="5" style="0" width="16.2"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="1" max="6" min="6" style="0" width="11.52"/>
@@ -4638,183 +4633,183 @@
       <c r="F1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="41"/>
-      <c r="L1" s="43" t="n">
+      <c r="K1" s="40"/>
+      <c r="L1" s="42" t="n">
         <v>44515</v>
       </c>
-      <c r="M1" s="43" t="n">
+      <c r="M1" s="42" t="n">
         <v>44516</v>
       </c>
-      <c r="N1" s="43" t="n">
+      <c r="N1" s="42" t="n">
         <v>44517</v>
       </c>
-      <c r="O1" s="43" t="n">
+      <c r="O1" s="42" t="n">
         <v>44518</v>
       </c>
-      <c r="P1" s="43" t="n">
+      <c r="P1" s="42" t="n">
         <v>44519</v>
       </c>
-      <c r="Q1" s="43" t="n">
+      <c r="Q1" s="42" t="n">
         <v>44520</v>
       </c>
-      <c r="R1" s="43" t="n">
+      <c r="R1" s="42" t="n">
         <v>44521</v>
       </c>
-      <c r="S1" s="43" t="n">
+      <c r="S1" s="42" t="n">
         <v>44522</v>
       </c>
-      <c r="T1" s="43" t="n">
+      <c r="T1" s="42" t="n">
         <v>44523</v>
       </c>
-      <c r="U1" s="43" t="n">
+      <c r="U1" s="42" t="n">
         <v>44524</v>
       </c>
-      <c r="V1" s="43" t="n">
+      <c r="V1" s="42" t="n">
         <v>44525</v>
       </c>
-      <c r="W1" s="43" t="n">
+      <c r="W1" s="42" t="n">
         <v>44526</v>
       </c>
-      <c r="X1" s="43" t="n">
+      <c r="X1" s="42" t="n">
         <v>44527</v>
       </c>
-      <c r="Y1" s="43" t="n">
+      <c r="Y1" s="42" t="n">
         <v>44528</v>
       </c>
-      <c r="Z1" s="43" t="n">
+      <c r="Z1" s="42" t="n">
         <v>44529</v>
       </c>
-      <c r="AA1" s="43" t="n">
+      <c r="AA1" s="42" t="n">
         <v>44530</v>
       </c>
-      <c r="AB1" s="43" t="n">
+      <c r="AB1" s="42" t="n">
         <v>44531</v>
       </c>
-      <c r="AC1" s="43" t="n">
+      <c r="AC1" s="42" t="n">
         <v>44532</v>
       </c>
-      <c r="AD1" s="43" t="n">
+      <c r="AD1" s="42" t="n">
         <v>44533</v>
       </c>
-      <c r="AE1" s="43" t="n">
+      <c r="AE1" s="42" t="n">
         <v>44534</v>
       </c>
-      <c r="AF1" s="43" t="n">
+      <c r="AF1" s="42" t="n">
         <v>44535</v>
       </c>
-      <c r="AG1" s="43" t="n">
+      <c r="AG1" s="42" t="n">
         <v>44536</v>
       </c>
-      <c r="AH1" s="43" t="n">
+      <c r="AH1" s="42" t="n">
         <v>44537</v>
       </c>
-      <c r="AI1" s="43" t="n">
+      <c r="AI1" s="42" t="n">
         <v>44538</v>
       </c>
-      <c r="AJ1" s="43" t="n">
+      <c r="AJ1" s="42" t="n">
         <v>44539</v>
       </c>
-      <c r="AK1" s="43" t="n">
+      <c r="AK1" s="42" t="n">
         <v>44540</v>
       </c>
-      <c r="AL1" s="43" t="n">
+      <c r="AL1" s="42" t="n">
         <v>44541</v>
       </c>
-      <c r="AM1" s="43" t="n">
+      <c r="AM1" s="42" t="n">
         <v>44542</v>
       </c>
-      <c r="AN1" s="43" t="n">
+      <c r="AN1" s="42" t="n">
         <v>44543</v>
       </c>
-      <c r="AO1" s="43" t="n">
+      <c r="AO1" s="42" t="n">
         <v>44544</v>
       </c>
-      <c r="AP1" s="43" t="n">
+      <c r="AP1" s="42" t="n">
         <v>44545</v>
       </c>
-      <c r="AQ1" s="43" t="n">
+      <c r="AQ1" s="42" t="n">
         <v>44546</v>
       </c>
-      <c r="AR1" s="43" t="n">
+      <c r="AR1" s="42" t="n">
         <v>44547</v>
       </c>
-      <c r="AS1" s="43" t="n">
+      <c r="AS1" s="42" t="n">
         <v>44548</v>
       </c>
-      <c r="AT1" s="43" t="n">
+      <c r="AT1" s="42" t="n">
         <v>44549</v>
       </c>
-      <c r="AU1" s="43" t="n">
+      <c r="AU1" s="42" t="n">
         <v>44550</v>
       </c>
-      <c r="AV1" s="43" t="n">
+      <c r="AV1" s="42" t="n">
         <v>44551</v>
       </c>
-      <c r="AW1" s="43" t="n">
+      <c r="AW1" s="42" t="n">
         <v>44552</v>
       </c>
-      <c r="AX1" s="43" t="n">
+      <c r="AX1" s="42" t="n">
         <v>44553</v>
       </c>
-      <c r="AY1" s="44" t="n">
+      <c r="AY1" s="43" t="n">
         <v>44554</v>
       </c>
-      <c r="AZ1" s="43" t="n">
+      <c r="AZ1" s="42" t="n">
         <v>44555</v>
       </c>
-      <c r="BA1" s="43" t="n">
+      <c r="BA1" s="42" t="n">
         <v>44556</v>
       </c>
-      <c r="BB1" s="43" t="n">
+      <c r="BB1" s="42" t="n">
         <v>44557</v>
       </c>
-      <c r="BC1" s="43" t="n">
+      <c r="BC1" s="42" t="n">
         <v>44558</v>
       </c>
-      <c r="BD1" s="43" t="n">
+      <c r="BD1" s="42" t="n">
         <v>44559</v>
       </c>
-      <c r="BE1" s="43" t="n">
+      <c r="BE1" s="42" t="n">
         <v>44560</v>
       </c>
-      <c r="BF1" s="44" t="n">
+      <c r="BF1" s="43" t="n">
         <v>44561</v>
       </c>
-      <c r="BG1" s="43" t="n">
+      <c r="BG1" s="42" t="n">
         <v>44562</v>
       </c>
-      <c r="BH1" s="43" t="n">
+      <c r="BH1" s="42" t="n">
         <v>44563</v>
       </c>
-      <c r="BI1" s="43" t="n">
+      <c r="BI1" s="42" t="n">
         <v>44564</v>
       </c>
-      <c r="BJ1" s="43" t="n">
+      <c r="BJ1" s="42" t="n">
         <v>44565</v>
       </c>
-      <c r="BK1" s="43" t="n">
+      <c r="BK1" s="42" t="n">
         <v>44566</v>
       </c>
-      <c r="BL1" s="44" t="n">
+      <c r="BL1" s="43" t="n">
         <v>44567</v>
       </c>
-      <c r="BM1" s="43" t="n">
+      <c r="BM1" s="42" t="n">
         <v>44568</v>
       </c>
       <c r="BN1" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4842,80 +4837,80 @@
         <f aca="false">Netzplan!I2</f>
         <v>1</v>
       </c>
-      <c r="J2" s="45" t="n">
+      <c r="J2" s="44" t="n">
         <f aca="false">Netzplan!J2</f>
         <v>5</v>
       </c>
-      <c r="K2" s="46" t="n">
+      <c r="K2" s="45" t="n">
         <f aca="false">SUM(L2:BM2)</f>
         <v>5</v>
       </c>
-      <c r="L2" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="48"/>
-      <c r="AC2" s="48"/>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48"/>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="48"/>
-      <c r="AI2" s="48"/>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-      <c r="AP2" s="48"/>
-      <c r="AQ2" s="48"/>
-      <c r="AR2" s="48"/>
-      <c r="AS2" s="48"/>
-      <c r="AT2" s="48"/>
-      <c r="AU2" s="48"/>
-      <c r="AV2" s="48"/>
-      <c r="AW2" s="48"/>
-      <c r="AX2" s="48"/>
-      <c r="AY2" s="49"/>
-      <c r="AZ2" s="48"/>
-      <c r="BA2" s="48"/>
-      <c r="BB2" s="48"/>
-      <c r="BC2" s="48"/>
-      <c r="BD2" s="48"/>
-      <c r="BE2" s="48"/>
-      <c r="BF2" s="49"/>
-      <c r="BG2" s="48"/>
-      <c r="BH2" s="48"/>
-      <c r="BI2" s="48"/>
-      <c r="BJ2" s="48"/>
-      <c r="BK2" s="48"/>
-      <c r="BL2" s="49"/>
-      <c r="BM2" s="48"/>
+      <c r="L2" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="47"/>
+      <c r="U2" s="47"/>
+      <c r="V2" s="47"/>
+      <c r="W2" s="47"/>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="47"/>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="47"/>
+      <c r="AC2" s="47"/>
+      <c r="AD2" s="47"/>
+      <c r="AE2" s="47"/>
+      <c r="AF2" s="47"/>
+      <c r="AG2" s="47"/>
+      <c r="AH2" s="47"/>
+      <c r="AI2" s="47"/>
+      <c r="AJ2" s="47"/>
+      <c r="AK2" s="47"/>
+      <c r="AL2" s="47"/>
+      <c r="AM2" s="47"/>
+      <c r="AN2" s="47"/>
+      <c r="AO2" s="47"/>
+      <c r="AP2" s="47"/>
+      <c r="AQ2" s="47"/>
+      <c r="AR2" s="47"/>
+      <c r="AS2" s="47"/>
+      <c r="AT2" s="47"/>
+      <c r="AU2" s="47"/>
+      <c r="AV2" s="47"/>
+      <c r="AW2" s="47"/>
+      <c r="AX2" s="47"/>
+      <c r="AY2" s="48"/>
+      <c r="AZ2" s="47"/>
+      <c r="BA2" s="47"/>
+      <c r="BB2" s="47"/>
+      <c r="BC2" s="47"/>
+      <c r="BD2" s="47"/>
+      <c r="BE2" s="47"/>
+      <c r="BF2" s="48"/>
+      <c r="BG2" s="47"/>
+      <c r="BH2" s="47"/>
+      <c r="BI2" s="47"/>
+      <c r="BJ2" s="47"/>
+      <c r="BK2" s="47"/>
+      <c r="BL2" s="48"/>
+      <c r="BM2" s="47"/>
       <c r="BN2" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4945,72 +4940,72 @@
         <f aca="false">Netzplan!I3</f>
         <v>1</v>
       </c>
-      <c r="J3" s="45" t="n">
+      <c r="J3" s="44" t="n">
         <f aca="false">Netzplan!J3</f>
         <v>1</v>
       </c>
-      <c r="K3" s="46" t="n">
+      <c r="K3" s="45" t="n">
         <f aca="false">SUM(L3:BM3)</f>
         <v>1</v>
       </c>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="T3" s="48"/>
-      <c r="U3" s="48"/>
-      <c r="V3" s="48"/>
-      <c r="W3" s="48"/>
-      <c r="X3" s="48"/>
-      <c r="Y3" s="48"/>
-      <c r="Z3" s="48"/>
-      <c r="AA3" s="48"/>
-      <c r="AB3" s="48"/>
-      <c r="AC3" s="48"/>
-      <c r="AD3" s="48"/>
-      <c r="AE3" s="48"/>
-      <c r="AF3" s="48"/>
-      <c r="AG3" s="48"/>
-      <c r="AH3" s="48"/>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="48"/>
-      <c r="AL3" s="48"/>
-      <c r="AM3" s="48"/>
-      <c r="AN3" s="48"/>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="48"/>
-      <c r="AQ3" s="48"/>
-      <c r="AR3" s="48"/>
-      <c r="AS3" s="48"/>
-      <c r="AT3" s="48"/>
-      <c r="AU3" s="48"/>
-      <c r="AV3" s="48"/>
-      <c r="AW3" s="48"/>
-      <c r="AX3" s="48"/>
-      <c r="AY3" s="49"/>
-      <c r="AZ3" s="48"/>
-      <c r="BA3" s="48"/>
-      <c r="BB3" s="48"/>
-      <c r="BC3" s="48"/>
-      <c r="BD3" s="48"/>
-      <c r="BE3" s="48"/>
-      <c r="BF3" s="49"/>
-      <c r="BG3" s="48"/>
-      <c r="BH3" s="48"/>
-      <c r="BI3" s="48"/>
-      <c r="BJ3" s="48"/>
-      <c r="BK3" s="48"/>
-      <c r="BL3" s="49"/>
-      <c r="BM3" s="48"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="47"/>
+      <c r="O3" s="47"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="47"/>
+      <c r="S3" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="47"/>
+      <c r="Y3" s="47"/>
+      <c r="Z3" s="47"/>
+      <c r="AA3" s="47"/>
+      <c r="AB3" s="47"/>
+      <c r="AC3" s="47"/>
+      <c r="AD3" s="47"/>
+      <c r="AE3" s="47"/>
+      <c r="AF3" s="47"/>
+      <c r="AG3" s="47"/>
+      <c r="AH3" s="47"/>
+      <c r="AI3" s="47"/>
+      <c r="AJ3" s="47"/>
+      <c r="AK3" s="47"/>
+      <c r="AL3" s="47"/>
+      <c r="AM3" s="47"/>
+      <c r="AN3" s="47"/>
+      <c r="AO3" s="47"/>
+      <c r="AP3" s="47"/>
+      <c r="AQ3" s="47"/>
+      <c r="AR3" s="47"/>
+      <c r="AS3" s="47"/>
+      <c r="AT3" s="47"/>
+      <c r="AU3" s="47"/>
+      <c r="AV3" s="47"/>
+      <c r="AW3" s="47"/>
+      <c r="AX3" s="47"/>
+      <c r="AY3" s="48"/>
+      <c r="AZ3" s="47"/>
+      <c r="BA3" s="47"/>
+      <c r="BB3" s="47"/>
+      <c r="BC3" s="47"/>
+      <c r="BD3" s="47"/>
+      <c r="BE3" s="47"/>
+      <c r="BF3" s="48"/>
+      <c r="BG3" s="47"/>
+      <c r="BH3" s="47"/>
+      <c r="BI3" s="47"/>
+      <c r="BJ3" s="47"/>
+      <c r="BK3" s="47"/>
+      <c r="BL3" s="48"/>
+      <c r="BM3" s="47"/>
       <c r="BN3" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5040,78 +5035,78 @@
         <f aca="false">Netzplan!I4</f>
         <v>1</v>
       </c>
-      <c r="J4" s="45" t="n">
+      <c r="J4" s="44" t="n">
         <f aca="false">Netzplan!J4</f>
         <v>4</v>
       </c>
-      <c r="K4" s="46" t="n">
+      <c r="K4" s="45" t="n">
         <f aca="false">SUM(L4:BM4)</f>
         <v>4</v>
       </c>
-      <c r="L4" s="48"/>
-      <c r="M4" s="48"/>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-      <c r="S4" s="48"/>
-      <c r="T4" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="U4" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="W4" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="X4" s="48"/>
-      <c r="Y4" s="48"/>
-      <c r="Z4" s="48"/>
-      <c r="AA4" s="48"/>
-      <c r="AB4" s="48"/>
-      <c r="AC4" s="48"/>
-      <c r="AD4" s="48"/>
-      <c r="AE4" s="48"/>
-      <c r="AF4" s="48"/>
-      <c r="AG4" s="48"/>
-      <c r="AH4" s="48"/>
-      <c r="AI4" s="48"/>
-      <c r="AJ4" s="48"/>
-      <c r="AK4" s="48"/>
-      <c r="AL4" s="48"/>
-      <c r="AM4" s="48"/>
-      <c r="AN4" s="48"/>
-      <c r="AO4" s="48"/>
-      <c r="AP4" s="48"/>
-      <c r="AQ4" s="48"/>
-      <c r="AR4" s="48"/>
-      <c r="AS4" s="48"/>
-      <c r="AT4" s="48"/>
-      <c r="AU4" s="48"/>
-      <c r="AV4" s="48"/>
-      <c r="AW4" s="48"/>
-      <c r="AX4" s="48"/>
-      <c r="AY4" s="49"/>
-      <c r="AZ4" s="48"/>
-      <c r="BA4" s="48"/>
-      <c r="BB4" s="48"/>
-      <c r="BC4" s="48"/>
-      <c r="BD4" s="48"/>
-      <c r="BE4" s="48"/>
-      <c r="BF4" s="49"/>
-      <c r="BG4" s="48"/>
-      <c r="BH4" s="48"/>
-      <c r="BI4" s="48"/>
-      <c r="BJ4" s="48"/>
-      <c r="BK4" s="48"/>
-      <c r="BL4" s="49"/>
-      <c r="BM4" s="48"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="47"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="47"/>
+      <c r="R4" s="47"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="47"/>
+      <c r="Y4" s="47"/>
+      <c r="Z4" s="47"/>
+      <c r="AA4" s="47"/>
+      <c r="AB4" s="47"/>
+      <c r="AC4" s="47"/>
+      <c r="AD4" s="47"/>
+      <c r="AE4" s="47"/>
+      <c r="AF4" s="47"/>
+      <c r="AG4" s="47"/>
+      <c r="AH4" s="47"/>
+      <c r="AI4" s="47"/>
+      <c r="AJ4" s="47"/>
+      <c r="AK4" s="47"/>
+      <c r="AL4" s="47"/>
+      <c r="AM4" s="47"/>
+      <c r="AN4" s="47"/>
+      <c r="AO4" s="47"/>
+      <c r="AP4" s="47"/>
+      <c r="AQ4" s="47"/>
+      <c r="AR4" s="47"/>
+      <c r="AS4" s="47"/>
+      <c r="AT4" s="47"/>
+      <c r="AU4" s="47"/>
+      <c r="AV4" s="47"/>
+      <c r="AW4" s="47"/>
+      <c r="AX4" s="47"/>
+      <c r="AY4" s="48"/>
+      <c r="AZ4" s="47"/>
+      <c r="BA4" s="47"/>
+      <c r="BB4" s="47"/>
+      <c r="BC4" s="47"/>
+      <c r="BD4" s="47"/>
+      <c r="BE4" s="47"/>
+      <c r="BF4" s="48"/>
+      <c r="BG4" s="47"/>
+      <c r="BH4" s="47"/>
+      <c r="BI4" s="47"/>
+      <c r="BJ4" s="47"/>
+      <c r="BK4" s="47"/>
+      <c r="BL4" s="48"/>
+      <c r="BM4" s="47"/>
       <c r="BN4" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5141,76 +5136,76 @@
         <f aca="false">Netzplan!I5</f>
         <v>1</v>
       </c>
-      <c r="J5" s="45" t="n">
+      <c r="J5" s="44" t="n">
         <f aca="false">Netzplan!J5</f>
         <v>3</v>
       </c>
-      <c r="K5" s="46" t="n">
+      <c r="K5" s="45" t="n">
         <f aca="false">SUM(L5:BM5)</f>
         <v>3</v>
       </c>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="48"/>
-      <c r="O5" s="48"/>
-      <c r="P5" s="48"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="V5" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="W5" s="48"/>
-      <c r="X5" s="48"/>
-      <c r="Y5" s="48"/>
-      <c r="Z5" s="48"/>
-      <c r="AA5" s="48"/>
-      <c r="AB5" s="48"/>
-      <c r="AC5" s="48"/>
-      <c r="AD5" s="48"/>
-      <c r="AE5" s="48"/>
-      <c r="AF5" s="48"/>
-      <c r="AG5" s="48"/>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="48"/>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="48"/>
-      <c r="AL5" s="48"/>
-      <c r="AM5" s="48"/>
-      <c r="AN5" s="48"/>
-      <c r="AO5" s="48"/>
-      <c r="AP5" s="48"/>
-      <c r="AQ5" s="48"/>
-      <c r="AR5" s="48"/>
-      <c r="AS5" s="48"/>
-      <c r="AT5" s="48"/>
-      <c r="AU5" s="48"/>
-      <c r="AV5" s="48"/>
-      <c r="AW5" s="48"/>
-      <c r="AX5" s="48"/>
-      <c r="AY5" s="49"/>
-      <c r="AZ5" s="48"/>
-      <c r="BA5" s="48"/>
-      <c r="BB5" s="48"/>
-      <c r="BC5" s="48"/>
-      <c r="BD5" s="48"/>
-      <c r="BE5" s="48"/>
-      <c r="BF5" s="49"/>
-      <c r="BG5" s="48"/>
-      <c r="BH5" s="48"/>
-      <c r="BI5" s="48"/>
-      <c r="BJ5" s="48"/>
-      <c r="BK5" s="48"/>
-      <c r="BL5" s="49"/>
-      <c r="BM5" s="48"/>
+      <c r="L5" s="47"/>
+      <c r="M5" s="47"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="47"/>
+      <c r="X5" s="47"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="47"/>
+      <c r="AA5" s="47"/>
+      <c r="AB5" s="47"/>
+      <c r="AC5" s="47"/>
+      <c r="AD5" s="47"/>
+      <c r="AE5" s="47"/>
+      <c r="AF5" s="47"/>
+      <c r="AG5" s="47"/>
+      <c r="AH5" s="47"/>
+      <c r="AI5" s="47"/>
+      <c r="AJ5" s="47"/>
+      <c r="AK5" s="47"/>
+      <c r="AL5" s="47"/>
+      <c r="AM5" s="47"/>
+      <c r="AN5" s="47"/>
+      <c r="AO5" s="47"/>
+      <c r="AP5" s="47"/>
+      <c r="AQ5" s="47"/>
+      <c r="AR5" s="47"/>
+      <c r="AS5" s="47"/>
+      <c r="AT5" s="47"/>
+      <c r="AU5" s="47"/>
+      <c r="AV5" s="47"/>
+      <c r="AW5" s="47"/>
+      <c r="AX5" s="47"/>
+      <c r="AY5" s="48"/>
+      <c r="AZ5" s="47"/>
+      <c r="BA5" s="47"/>
+      <c r="BB5" s="47"/>
+      <c r="BC5" s="47"/>
+      <c r="BD5" s="47"/>
+      <c r="BE5" s="47"/>
+      <c r="BF5" s="48"/>
+      <c r="BG5" s="47"/>
+      <c r="BH5" s="47"/>
+      <c r="BI5" s="47"/>
+      <c r="BJ5" s="47"/>
+      <c r="BK5" s="47"/>
+      <c r="BL5" s="48"/>
+      <c r="BM5" s="47"/>
       <c r="BN5" s="0" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5234,86 +5229,86 @@
       </c>
       <c r="H6" s="30" t="str">
         <f aca="false">Netzplan!H6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I6" s="31" t="n">
         <f aca="false">Netzplan!I6</f>
-        <v>0.75</v>
-      </c>
-      <c r="J6" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="44" t="n">
         <f aca="false">Netzplan!J6</f>
-        <v>5</v>
-      </c>
-      <c r="K6" s="46" t="n">
+        <v>7</v>
+      </c>
+      <c r="K6" s="45" t="n">
         <f aca="false">SUM(L6:BM6)</f>
         <v>5</v>
       </c>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
-      <c r="O6" s="48"/>
-      <c r="P6" s="48"/>
-      <c r="Q6" s="48"/>
-      <c r="R6" s="48"/>
-      <c r="S6" s="48"/>
-      <c r="T6" s="48"/>
-      <c r="U6" s="48"/>
-      <c r="V6" s="48"/>
-      <c r="W6" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="X6" s="48"/>
-      <c r="Y6" s="48"/>
-      <c r="Z6" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="48"/>
-      <c r="AE6" s="48"/>
-      <c r="AF6" s="48"/>
-      <c r="AG6" s="48"/>
-      <c r="AH6" s="48"/>
-      <c r="AI6" s="48"/>
-      <c r="AJ6" s="48"/>
-      <c r="AK6" s="48"/>
-      <c r="AL6" s="48"/>
-      <c r="AM6" s="48"/>
-      <c r="AN6" s="48"/>
-      <c r="AO6" s="48"/>
-      <c r="AP6" s="48"/>
-      <c r="AQ6" s="48"/>
-      <c r="AR6" s="48"/>
-      <c r="AS6" s="48"/>
-      <c r="AT6" s="48"/>
-      <c r="AU6" s="48"/>
-      <c r="AV6" s="48"/>
-      <c r="AW6" s="48"/>
-      <c r="AX6" s="48"/>
-      <c r="AY6" s="49"/>
-      <c r="AZ6" s="48"/>
-      <c r="BA6" s="48"/>
-      <c r="BB6" s="48"/>
-      <c r="BC6" s="48"/>
-      <c r="BD6" s="48"/>
-      <c r="BE6" s="48"/>
-      <c r="BF6" s="49"/>
-      <c r="BG6" s="48"/>
-      <c r="BH6" s="48"/>
-      <c r="BI6" s="48"/>
-      <c r="BJ6" s="48"/>
-      <c r="BK6" s="48"/>
-      <c r="BL6" s="49"/>
-      <c r="BM6" s="48"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="47"/>
+      <c r="R6" s="47"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="V6" s="47"/>
+      <c r="W6" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="47"/>
+      <c r="Y6" s="47"/>
+      <c r="Z6" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="47"/>
+      <c r="AE6" s="47"/>
+      <c r="AF6" s="47"/>
+      <c r="AG6" s="47"/>
+      <c r="AH6" s="47"/>
+      <c r="AI6" s="47"/>
+      <c r="AJ6" s="47"/>
+      <c r="AK6" s="47"/>
+      <c r="AL6" s="47"/>
+      <c r="AM6" s="47"/>
+      <c r="AN6" s="47"/>
+      <c r="AO6" s="47"/>
+      <c r="AP6" s="47"/>
+      <c r="AQ6" s="47"/>
+      <c r="AR6" s="47"/>
+      <c r="AS6" s="47"/>
+      <c r="AT6" s="47"/>
+      <c r="AU6" s="47"/>
+      <c r="AV6" s="47"/>
+      <c r="AW6" s="47"/>
+      <c r="AX6" s="47"/>
+      <c r="AY6" s="48"/>
+      <c r="AZ6" s="47"/>
+      <c r="BA6" s="47"/>
+      <c r="BB6" s="47"/>
+      <c r="BC6" s="47"/>
+      <c r="BD6" s="47"/>
+      <c r="BE6" s="47"/>
+      <c r="BF6" s="48"/>
+      <c r="BG6" s="47"/>
+      <c r="BH6" s="47"/>
+      <c r="BI6" s="47"/>
+      <c r="BJ6" s="47"/>
+      <c r="BK6" s="47"/>
+      <c r="BL6" s="48"/>
+      <c r="BM6" s="47"/>
       <c r="BN6" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5343,72 +5338,72 @@
         <f aca="false">Netzplan!I7</f>
         <v>1</v>
       </c>
-      <c r="J7" s="45" t="n">
+      <c r="J7" s="44" t="n">
         <f aca="false">Netzplan!J7</f>
         <v>1</v>
       </c>
-      <c r="K7" s="46" t="n">
+      <c r="K7" s="45" t="n">
         <f aca="false">SUM(L7:BM7)</f>
         <v>1</v>
       </c>
-      <c r="L7" s="48"/>
-      <c r="M7" s="48"/>
-      <c r="N7" s="48"/>
-      <c r="O7" s="48"/>
-      <c r="P7" s="48"/>
-      <c r="Q7" s="48"/>
-      <c r="R7" s="48"/>
-      <c r="S7" s="50"/>
-      <c r="T7" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="U7" s="48"/>
-      <c r="V7" s="48"/>
-      <c r="W7" s="48"/>
-      <c r="X7" s="48"/>
-      <c r="Y7" s="48"/>
-      <c r="Z7" s="48"/>
-      <c r="AA7" s="48"/>
-      <c r="AB7" s="48"/>
-      <c r="AC7" s="48"/>
-      <c r="AD7" s="48"/>
-      <c r="AE7" s="48"/>
-      <c r="AF7" s="48"/>
-      <c r="AG7" s="48"/>
-      <c r="AH7" s="48"/>
-      <c r="AI7" s="48"/>
-      <c r="AJ7" s="48"/>
-      <c r="AK7" s="48"/>
-      <c r="AL7" s="48"/>
-      <c r="AM7" s="48"/>
-      <c r="AN7" s="48"/>
-      <c r="AO7" s="48"/>
-      <c r="AP7" s="48"/>
-      <c r="AQ7" s="48"/>
-      <c r="AR7" s="48"/>
-      <c r="AS7" s="48"/>
-      <c r="AT7" s="48"/>
-      <c r="AU7" s="48"/>
-      <c r="AV7" s="48"/>
-      <c r="AW7" s="48"/>
-      <c r="AX7" s="48"/>
-      <c r="AY7" s="49"/>
-      <c r="AZ7" s="48"/>
-      <c r="BA7" s="48"/>
-      <c r="BB7" s="51"/>
-      <c r="BC7" s="51"/>
-      <c r="BD7" s="51"/>
-      <c r="BE7" s="51"/>
-      <c r="BF7" s="49"/>
-      <c r="BG7" s="48"/>
-      <c r="BH7" s="48"/>
-      <c r="BI7" s="48"/>
-      <c r="BJ7" s="48"/>
-      <c r="BK7" s="48"/>
-      <c r="BL7" s="49"/>
-      <c r="BM7" s="48"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
+      <c r="S7" s="49"/>
+      <c r="T7" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="U7" s="47"/>
+      <c r="V7" s="47"/>
+      <c r="W7" s="47"/>
+      <c r="X7" s="47"/>
+      <c r="Y7" s="47"/>
+      <c r="Z7" s="47"/>
+      <c r="AA7" s="47"/>
+      <c r="AB7" s="47"/>
+      <c r="AC7" s="47"/>
+      <c r="AD7" s="47"/>
+      <c r="AE7" s="47"/>
+      <c r="AF7" s="47"/>
+      <c r="AG7" s="47"/>
+      <c r="AH7" s="47"/>
+      <c r="AI7" s="47"/>
+      <c r="AJ7" s="47"/>
+      <c r="AK7" s="47"/>
+      <c r="AL7" s="47"/>
+      <c r="AM7" s="47"/>
+      <c r="AN7" s="47"/>
+      <c r="AO7" s="47"/>
+      <c r="AP7" s="47"/>
+      <c r="AQ7" s="47"/>
+      <c r="AR7" s="47"/>
+      <c r="AS7" s="47"/>
+      <c r="AT7" s="47"/>
+      <c r="AU7" s="47"/>
+      <c r="AV7" s="47"/>
+      <c r="AW7" s="47"/>
+      <c r="AX7" s="47"/>
+      <c r="AY7" s="48"/>
+      <c r="AZ7" s="47"/>
+      <c r="BA7" s="47"/>
+      <c r="BB7" s="50"/>
+      <c r="BC7" s="50"/>
+      <c r="BD7" s="50"/>
+      <c r="BE7" s="50"/>
+      <c r="BF7" s="48"/>
+      <c r="BG7" s="47"/>
+      <c r="BH7" s="47"/>
+      <c r="BI7" s="47"/>
+      <c r="BJ7" s="47"/>
+      <c r="BK7" s="47"/>
+      <c r="BL7" s="48"/>
+      <c r="BM7" s="47"/>
       <c r="BN7" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5424,7 +5419,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="30" t="n">
         <f aca="false">Netzplan!G8</f>
@@ -5438,82 +5433,82 @@
         <f aca="false">Netzplan!I8</f>
         <v>1</v>
       </c>
-      <c r="J8" s="45" t="n">
+      <c r="J8" s="44" t="n">
         <f aca="false">Netzplan!J8</f>
         <v>3</v>
       </c>
-      <c r="K8" s="46" t="n">
+      <c r="K8" s="45" t="n">
         <f aca="false">SUM(L8:BM8)</f>
         <v>3</v>
       </c>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="47"/>
-      <c r="U8" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="V8" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="W8" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="X8" s="48"/>
-      <c r="Y8" s="48"/>
-      <c r="Z8" s="48"/>
-      <c r="AA8" s="48"/>
-      <c r="AB8" s="48"/>
-      <c r="AC8" s="48"/>
-      <c r="AD8" s="48"/>
-      <c r="AE8" s="48"/>
-      <c r="AF8" s="48"/>
-      <c r="AG8" s="48"/>
-      <c r="AH8" s="48"/>
-      <c r="AI8" s="48"/>
-      <c r="AJ8" s="48"/>
-      <c r="AK8" s="48"/>
-      <c r="AL8" s="48"/>
-      <c r="AM8" s="48"/>
-      <c r="AN8" s="48"/>
-      <c r="AO8" s="48"/>
-      <c r="AP8" s="48"/>
-      <c r="AQ8" s="48"/>
-      <c r="AR8" s="48"/>
-      <c r="AS8" s="48"/>
-      <c r="AT8" s="48"/>
-      <c r="AU8" s="48"/>
-      <c r="AV8" s="48"/>
-      <c r="AW8" s="48"/>
-      <c r="AX8" s="48"/>
-      <c r="AY8" s="49"/>
-      <c r="AZ8" s="48"/>
-      <c r="BA8" s="48"/>
-      <c r="BB8" s="48"/>
-      <c r="BC8" s="48"/>
-      <c r="BD8" s="48"/>
-      <c r="BE8" s="48"/>
-      <c r="BF8" s="49"/>
-      <c r="BG8" s="48"/>
-      <c r="BH8" s="48"/>
-      <c r="BI8" s="48"/>
-      <c r="BJ8" s="48"/>
-      <c r="BK8" s="48"/>
-      <c r="BL8" s="49"/>
-      <c r="BM8" s="48"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
+      <c r="S8" s="47"/>
+      <c r="T8" s="46"/>
+      <c r="U8" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="V8" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="W8" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="X8" s="47"/>
+      <c r="Y8" s="47"/>
+      <c r="Z8" s="47"/>
+      <c r="AA8" s="47"/>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="47"/>
+      <c r="AD8" s="47"/>
+      <c r="AE8" s="47"/>
+      <c r="AF8" s="47"/>
+      <c r="AG8" s="47"/>
+      <c r="AH8" s="47"/>
+      <c r="AI8" s="47"/>
+      <c r="AJ8" s="47"/>
+      <c r="AK8" s="47"/>
+      <c r="AL8" s="47"/>
+      <c r="AM8" s="47"/>
+      <c r="AN8" s="47"/>
+      <c r="AO8" s="47"/>
+      <c r="AP8" s="47"/>
+      <c r="AQ8" s="47"/>
+      <c r="AR8" s="47"/>
+      <c r="AS8" s="47"/>
+      <c r="AT8" s="47"/>
+      <c r="AU8" s="47"/>
+      <c r="AV8" s="47"/>
+      <c r="AW8" s="47"/>
+      <c r="AX8" s="47"/>
+      <c r="AY8" s="48"/>
+      <c r="AZ8" s="47"/>
+      <c r="BA8" s="47"/>
+      <c r="BB8" s="47"/>
+      <c r="BC8" s="47"/>
+      <c r="BD8" s="47"/>
+      <c r="BE8" s="47"/>
+      <c r="BF8" s="48"/>
+      <c r="BG8" s="47"/>
+      <c r="BH8" s="47"/>
+      <c r="BI8" s="47"/>
+      <c r="BJ8" s="47"/>
+      <c r="BK8" s="47"/>
+      <c r="BL8" s="48"/>
+      <c r="BM8" s="47"/>
       <c r="BN8" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14"/>
       <c r="B9" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="36"/>
@@ -5522,64 +5517,64 @@
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
       <c r="I9" s="31"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="46"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="48"/>
-      <c r="S9" s="48"/>
-      <c r="T9" s="47"/>
-      <c r="U9" s="47"/>
-      <c r="V9" s="47"/>
-      <c r="W9" s="48"/>
-      <c r="X9" s="48"/>
-      <c r="Y9" s="48"/>
-      <c r="Z9" s="48"/>
-      <c r="AA9" s="48"/>
-      <c r="AB9" s="48"/>
-      <c r="AC9" s="48"/>
-      <c r="AD9" s="48"/>
-      <c r="AE9" s="48"/>
-      <c r="AF9" s="48"/>
-      <c r="AG9" s="48"/>
-      <c r="AH9" s="48"/>
-      <c r="AI9" s="48"/>
-      <c r="AJ9" s="48"/>
-      <c r="AK9" s="48"/>
-      <c r="AL9" s="48"/>
-      <c r="AM9" s="48"/>
-      <c r="AN9" s="48"/>
-      <c r="AO9" s="48"/>
-      <c r="AP9" s="48"/>
-      <c r="AQ9" s="48"/>
-      <c r="AR9" s="48"/>
-      <c r="AS9" s="48"/>
-      <c r="AT9" s="48"/>
-      <c r="AU9" s="48"/>
-      <c r="AV9" s="48"/>
-      <c r="AW9" s="48"/>
-      <c r="AX9" s="48"/>
-      <c r="AY9" s="49"/>
-      <c r="AZ9" s="48"/>
-      <c r="BA9" s="48"/>
-      <c r="BB9" s="48"/>
-      <c r="BC9" s="48"/>
-      <c r="BD9" s="48"/>
-      <c r="BE9" s="48"/>
-      <c r="BF9" s="49"/>
-      <c r="BG9" s="48"/>
-      <c r="BH9" s="48"/>
-      <c r="BI9" s="48"/>
-      <c r="BJ9" s="48"/>
-      <c r="BK9" s="48"/>
-      <c r="BL9" s="49"/>
-      <c r="BM9" s="48"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="46"/>
+      <c r="U9" s="46"/>
+      <c r="V9" s="46"/>
+      <c r="W9" s="47"/>
+      <c r="X9" s="47"/>
+      <c r="Y9" s="47"/>
+      <c r="Z9" s="47"/>
+      <c r="AA9" s="47"/>
+      <c r="AB9" s="47"/>
+      <c r="AC9" s="47"/>
+      <c r="AD9" s="47"/>
+      <c r="AE9" s="47"/>
+      <c r="AF9" s="47"/>
+      <c r="AG9" s="47"/>
+      <c r="AH9" s="47"/>
+      <c r="AI9" s="47"/>
+      <c r="AJ9" s="47"/>
+      <c r="AK9" s="47"/>
+      <c r="AL9" s="47"/>
+      <c r="AM9" s="47"/>
+      <c r="AN9" s="47"/>
+      <c r="AO9" s="47"/>
+      <c r="AP9" s="47"/>
+      <c r="AQ9" s="47"/>
+      <c r="AR9" s="47"/>
+      <c r="AS9" s="47"/>
+      <c r="AT9" s="47"/>
+      <c r="AU9" s="47"/>
+      <c r="AV9" s="47"/>
+      <c r="AW9" s="47"/>
+      <c r="AX9" s="47"/>
+      <c r="AY9" s="48"/>
+      <c r="AZ9" s="47"/>
+      <c r="BA9" s="47"/>
+      <c r="BB9" s="47"/>
+      <c r="BC9" s="47"/>
+      <c r="BD9" s="47"/>
+      <c r="BE9" s="47"/>
+      <c r="BF9" s="48"/>
+      <c r="BG9" s="47"/>
+      <c r="BH9" s="47"/>
+      <c r="BI9" s="47"/>
+      <c r="BJ9" s="47"/>
+      <c r="BK9" s="47"/>
+      <c r="BL9" s="48"/>
+      <c r="BM9" s="47"/>
       <c r="BN9" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5592,7 +5587,7 @@
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
       <c r="E10" s="35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F10" s="35" t="s">
         <v>35</v>
@@ -5609,74 +5604,74 @@
         <f aca="false">Netzplan!I9</f>
         <v>1</v>
       </c>
-      <c r="J10" s="45" t="n">
+      <c r="J10" s="44" t="n">
         <f aca="false">Netzplan!J9</f>
         <v>2</v>
       </c>
-      <c r="K10" s="46" t="n">
+      <c r="K10" s="45" t="n">
         <f aca="false">SUM(L10:BM10)</f>
         <v>2</v>
       </c>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="48"/>
-      <c r="S10" s="48"/>
-      <c r="T10" s="48"/>
-      <c r="U10" s="48"/>
-      <c r="V10" s="48"/>
-      <c r="W10" s="48"/>
-      <c r="X10" s="48"/>
-      <c r="Y10" s="48"/>
-      <c r="Z10" s="48"/>
-      <c r="AA10" s="48"/>
-      <c r="AB10" s="48"/>
-      <c r="AC10" s="48"/>
-      <c r="AD10" s="47"/>
-      <c r="AE10" s="48"/>
-      <c r="AF10" s="48"/>
-      <c r="AG10" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH10" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI10" s="48"/>
-      <c r="AJ10" s="48"/>
-      <c r="AK10" s="48"/>
-      <c r="AL10" s="48"/>
-      <c r="AM10" s="48"/>
-      <c r="AN10" s="48"/>
-      <c r="AO10" s="48"/>
-      <c r="AP10" s="48"/>
-      <c r="AQ10" s="48"/>
-      <c r="AR10" s="48"/>
-      <c r="AS10" s="48"/>
-      <c r="AT10" s="48"/>
-      <c r="AU10" s="48"/>
-      <c r="AV10" s="48"/>
-      <c r="AW10" s="48"/>
-      <c r="AX10" s="48"/>
-      <c r="AY10" s="49"/>
-      <c r="AZ10" s="48"/>
-      <c r="BA10" s="48"/>
-      <c r="BB10" s="48"/>
-      <c r="BC10" s="48"/>
-      <c r="BD10" s="48"/>
-      <c r="BE10" s="48"/>
-      <c r="BF10" s="49"/>
-      <c r="BG10" s="48"/>
-      <c r="BH10" s="48"/>
-      <c r="BI10" s="48"/>
-      <c r="BJ10" s="48"/>
-      <c r="BK10" s="48"/>
-      <c r="BL10" s="49"/>
-      <c r="BM10" s="48"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="47"/>
+      <c r="W10" s="47"/>
+      <c r="X10" s="47"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="47"/>
+      <c r="AA10" s="47"/>
+      <c r="AB10" s="47"/>
+      <c r="AC10" s="47"/>
+      <c r="AD10" s="46"/>
+      <c r="AE10" s="47"/>
+      <c r="AF10" s="47"/>
+      <c r="AG10" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI10" s="47"/>
+      <c r="AJ10" s="47"/>
+      <c r="AK10" s="47"/>
+      <c r="AL10" s="47"/>
+      <c r="AM10" s="47"/>
+      <c r="AN10" s="47"/>
+      <c r="AO10" s="47"/>
+      <c r="AP10" s="47"/>
+      <c r="AQ10" s="47"/>
+      <c r="AR10" s="47"/>
+      <c r="AS10" s="47"/>
+      <c r="AT10" s="47"/>
+      <c r="AU10" s="47"/>
+      <c r="AV10" s="47"/>
+      <c r="AW10" s="47"/>
+      <c r="AX10" s="47"/>
+      <c r="AY10" s="48"/>
+      <c r="AZ10" s="47"/>
+      <c r="BA10" s="47"/>
+      <c r="BB10" s="47"/>
+      <c r="BC10" s="47"/>
+      <c r="BD10" s="47"/>
+      <c r="BE10" s="47"/>
+      <c r="BF10" s="48"/>
+      <c r="BG10" s="47"/>
+      <c r="BH10" s="47"/>
+      <c r="BI10" s="47"/>
+      <c r="BJ10" s="47"/>
+      <c r="BK10" s="47"/>
+      <c r="BL10" s="48"/>
+      <c r="BM10" s="47"/>
       <c r="BN10" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5706,74 +5701,74 @@
         <f aca="false">Netzplan!I10</f>
         <v>1</v>
       </c>
-      <c r="J11" s="45" t="n">
+      <c r="J11" s="44" t="n">
         <f aca="false">Netzplan!J10</f>
         <v>2</v>
       </c>
-      <c r="K11" s="46" t="n">
+      <c r="K11" s="45" t="n">
         <f aca="false">SUM(L11:BM11)</f>
         <v>2</v>
       </c>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="48"/>
-      <c r="W11" s="48"/>
-      <c r="X11" s="48"/>
-      <c r="Y11" s="48"/>
-      <c r="Z11" s="48"/>
-      <c r="AA11" s="48"/>
-      <c r="AB11" s="48"/>
-      <c r="AC11" s="48"/>
-      <c r="AD11" s="48"/>
-      <c r="AE11" s="48"/>
-      <c r="AF11" s="48"/>
-      <c r="AG11" s="48"/>
-      <c r="AH11" s="47"/>
-      <c r="AI11" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ11" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK11" s="48"/>
-      <c r="AL11" s="48"/>
-      <c r="AM11" s="48"/>
-      <c r="AN11" s="48"/>
-      <c r="AO11" s="48"/>
-      <c r="AP11" s="48"/>
-      <c r="AQ11" s="48"/>
-      <c r="AR11" s="48"/>
-      <c r="AS11" s="48"/>
-      <c r="AT11" s="48"/>
-      <c r="AU11" s="48"/>
-      <c r="AV11" s="48"/>
-      <c r="AW11" s="48"/>
-      <c r="AX11" s="48"/>
-      <c r="AY11" s="49"/>
-      <c r="AZ11" s="48"/>
-      <c r="BA11" s="48"/>
-      <c r="BB11" s="48"/>
-      <c r="BC11" s="48"/>
-      <c r="BD11" s="48"/>
-      <c r="BE11" s="48"/>
-      <c r="BF11" s="49"/>
-      <c r="BG11" s="48"/>
-      <c r="BH11" s="48"/>
-      <c r="BI11" s="48"/>
-      <c r="BJ11" s="48"/>
-      <c r="BK11" s="48"/>
-      <c r="BL11" s="49"/>
-      <c r="BM11" s="48"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="47"/>
+      <c r="R11" s="47"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="V11" s="47"/>
+      <c r="W11" s="47"/>
+      <c r="X11" s="47"/>
+      <c r="Y11" s="47"/>
+      <c r="Z11" s="47"/>
+      <c r="AA11" s="47"/>
+      <c r="AB11" s="47"/>
+      <c r="AC11" s="47"/>
+      <c r="AD11" s="47"/>
+      <c r="AE11" s="47"/>
+      <c r="AF11" s="47"/>
+      <c r="AG11" s="47"/>
+      <c r="AH11" s="46"/>
+      <c r="AI11" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK11" s="47"/>
+      <c r="AL11" s="47"/>
+      <c r="AM11" s="47"/>
+      <c r="AN11" s="47"/>
+      <c r="AO11" s="47"/>
+      <c r="AP11" s="47"/>
+      <c r="AQ11" s="47"/>
+      <c r="AR11" s="47"/>
+      <c r="AS11" s="47"/>
+      <c r="AT11" s="47"/>
+      <c r="AU11" s="47"/>
+      <c r="AV11" s="47"/>
+      <c r="AW11" s="47"/>
+      <c r="AX11" s="47"/>
+      <c r="AY11" s="48"/>
+      <c r="AZ11" s="47"/>
+      <c r="BA11" s="47"/>
+      <c r="BB11" s="47"/>
+      <c r="BC11" s="47"/>
+      <c r="BD11" s="47"/>
+      <c r="BE11" s="47"/>
+      <c r="BF11" s="48"/>
+      <c r="BG11" s="47"/>
+      <c r="BH11" s="47"/>
+      <c r="BI11" s="47"/>
+      <c r="BJ11" s="47"/>
+      <c r="BK11" s="47"/>
+      <c r="BL11" s="48"/>
+      <c r="BM11" s="47"/>
       <c r="BN11" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5803,73 +5798,73 @@
         <f aca="false">Netzplan!I11</f>
         <v>1</v>
       </c>
-      <c r="J12" s="45" t="n">
+      <c r="J12" s="44" t="n">
         <f aca="false">Netzplan!J11</f>
         <v>2</v>
       </c>
-      <c r="K12" s="46" t="n">
+      <c r="K12" s="45" t="n">
         <f aca="false">SUM(L12:BM12)</f>
         <v>2</v>
       </c>
-      <c r="L12" s="48"/>
-      <c r="M12" s="48"/>
-      <c r="N12" s="48"/>
-      <c r="O12" s="48"/>
-      <c r="P12" s="48"/>
-      <c r="Q12" s="48"/>
-      <c r="R12" s="48"/>
-      <c r="S12" s="48"/>
-      <c r="T12" s="48"/>
-      <c r="U12" s="48"/>
-      <c r="V12" s="48"/>
-      <c r="W12" s="48"/>
-      <c r="X12" s="48"/>
-      <c r="Y12" s="48"/>
-      <c r="Z12" s="48"/>
-      <c r="AA12" s="48"/>
-      <c r="AB12" s="48"/>
-      <c r="AC12" s="48"/>
-      <c r="AD12" s="48"/>
-      <c r="AE12" s="48"/>
-      <c r="AF12" s="48"/>
-      <c r="AG12" s="48"/>
-      <c r="AH12" s="48"/>
-      <c r="AJ12" s="47"/>
-      <c r="AK12" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL12" s="48"/>
-      <c r="AM12" s="48"/>
-      <c r="AN12" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO12" s="48"/>
-      <c r="AP12" s="48"/>
-      <c r="AQ12" s="48"/>
-      <c r="AR12" s="48"/>
-      <c r="AS12" s="48"/>
-      <c r="AT12" s="48"/>
-      <c r="AU12" s="48"/>
-      <c r="AV12" s="48"/>
-      <c r="AW12" s="48"/>
-      <c r="AX12" s="48"/>
-      <c r="AY12" s="49"/>
-      <c r="AZ12" s="48"/>
-      <c r="BA12" s="48"/>
-      <c r="BB12" s="48"/>
-      <c r="BC12" s="48"/>
-      <c r="BD12" s="48"/>
-      <c r="BE12" s="48"/>
-      <c r="BF12" s="49"/>
-      <c r="BG12" s="48"/>
-      <c r="BH12" s="48"/>
-      <c r="BI12" s="48"/>
-      <c r="BJ12" s="48"/>
-      <c r="BK12" s="48"/>
-      <c r="BL12" s="49"/>
-      <c r="BM12" s="48"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="47"/>
+      <c r="O12" s="47"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="47"/>
+      <c r="R12" s="47"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="V12" s="47"/>
+      <c r="W12" s="47"/>
+      <c r="X12" s="47"/>
+      <c r="Y12" s="47"/>
+      <c r="Z12" s="47"/>
+      <c r="AA12" s="47"/>
+      <c r="AB12" s="47"/>
+      <c r="AC12" s="47"/>
+      <c r="AD12" s="47"/>
+      <c r="AE12" s="47"/>
+      <c r="AF12" s="47"/>
+      <c r="AG12" s="47"/>
+      <c r="AH12" s="47"/>
+      <c r="AJ12" s="46"/>
+      <c r="AK12" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL12" s="47"/>
+      <c r="AM12" s="47"/>
+      <c r="AN12" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO12" s="47"/>
+      <c r="AP12" s="47"/>
+      <c r="AQ12" s="47"/>
+      <c r="AR12" s="47"/>
+      <c r="AS12" s="47"/>
+      <c r="AT12" s="47"/>
+      <c r="AU12" s="47"/>
+      <c r="AV12" s="47"/>
+      <c r="AW12" s="47"/>
+      <c r="AX12" s="47"/>
+      <c r="AY12" s="48"/>
+      <c r="AZ12" s="47"/>
+      <c r="BA12" s="47"/>
+      <c r="BB12" s="47"/>
+      <c r="BC12" s="47"/>
+      <c r="BD12" s="47"/>
+      <c r="BE12" s="47"/>
+      <c r="BF12" s="48"/>
+      <c r="BG12" s="47"/>
+      <c r="BH12" s="47"/>
+      <c r="BI12" s="47"/>
+      <c r="BJ12" s="47"/>
+      <c r="BK12" s="47"/>
+      <c r="BL12" s="48"/>
+      <c r="BM12" s="47"/>
       <c r="BN12" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5877,7 +5872,7 @@
         <v>17</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -5897,117 +5892,117 @@
       </c>
       <c r="I13" s="31" t="n">
         <f aca="false">Netzplan!I12</f>
-        <v>0.5</v>
-      </c>
-      <c r="J13" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="44" t="n">
         <f aca="false">Netzplan!J12</f>
-        <v>20</v>
-      </c>
-      <c r="K13" s="46" t="n">
+        <v>10</v>
+      </c>
+      <c r="K13" s="45" t="n">
         <f aca="false">SUM(L13:BM13)</f>
         <v>20</v>
       </c>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-      <c r="U13" s="48"/>
-      <c r="V13" s="48"/>
-      <c r="W13" s="47"/>
-      <c r="X13" s="48"/>
-      <c r="Y13" s="48"/>
-      <c r="Z13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="48"/>
-      <c r="AF13" s="48"/>
-      <c r="AG13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL13" s="48"/>
-      <c r="AM13" s="48"/>
-      <c r="AN13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS13" s="48"/>
-      <c r="AT13" s="48"/>
-      <c r="AU13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX13" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY13" s="49"/>
-      <c r="AZ13" s="48"/>
-      <c r="BA13" s="48"/>
-      <c r="BB13" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC13" s="48"/>
-      <c r="BD13" s="48"/>
-      <c r="BE13" s="48"/>
-      <c r="BF13" s="49"/>
-      <c r="BG13" s="48"/>
-      <c r="BH13" s="48"/>
-      <c r="BJ13" s="48"/>
-      <c r="BK13" s="48"/>
-      <c r="BL13" s="49"/>
-      <c r="BM13" s="48"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="47"/>
+      <c r="W13" s="46"/>
+      <c r="X13" s="47"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="47"/>
+      <c r="AF13" s="47"/>
+      <c r="AG13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="47"/>
+      <c r="AM13" s="47"/>
+      <c r="AN13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS13" s="47"/>
+      <c r="AT13" s="47"/>
+      <c r="AU13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX13" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY13" s="48"/>
+      <c r="AZ13" s="47"/>
+      <c r="BA13" s="47"/>
+      <c r="BB13" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC13" s="47"/>
+      <c r="BD13" s="47"/>
+      <c r="BE13" s="47"/>
+      <c r="BF13" s="48"/>
+      <c r="BG13" s="47"/>
+      <c r="BH13" s="47"/>
+      <c r="BJ13" s="47"/>
+      <c r="BK13" s="47"/>
+      <c r="BL13" s="48"/>
+      <c r="BM13" s="47"/>
       <c r="BN13" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14"/>
       <c r="B14" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
@@ -6016,63 +6011,63 @@
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
       <c r="I14" s="31"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="48"/>
-      <c r="U14" s="48"/>
-      <c r="V14" s="48"/>
-      <c r="W14" s="47"/>
-      <c r="X14" s="48"/>
-      <c r="Y14" s="48"/>
-      <c r="Z14" s="47"/>
-      <c r="AA14" s="47"/>
-      <c r="AB14" s="47"/>
-      <c r="AC14" s="47"/>
-      <c r="AD14" s="47"/>
-      <c r="AE14" s="48"/>
-      <c r="AF14" s="48"/>
-      <c r="AG14" s="47"/>
-      <c r="AH14" s="47"/>
-      <c r="AI14" s="47"/>
-      <c r="AJ14" s="47"/>
-      <c r="AK14" s="47"/>
-      <c r="AL14" s="48"/>
-      <c r="AM14" s="48"/>
-      <c r="AN14" s="47"/>
-      <c r="AO14" s="47"/>
-      <c r="AP14" s="47"/>
-      <c r="AQ14" s="47"/>
-      <c r="AR14" s="47"/>
-      <c r="AS14" s="48"/>
-      <c r="AT14" s="48"/>
-      <c r="AU14" s="47"/>
-      <c r="AV14" s="47"/>
-      <c r="AW14" s="47"/>
-      <c r="AX14" s="47"/>
-      <c r="AY14" s="49"/>
-      <c r="AZ14" s="48"/>
-      <c r="BA14" s="48"/>
-      <c r="BB14" s="48"/>
-      <c r="BC14" s="48"/>
-      <c r="BD14" s="48"/>
-      <c r="BE14" s="48"/>
-      <c r="BF14" s="49"/>
-      <c r="BG14" s="48"/>
-      <c r="BH14" s="48"/>
-      <c r="BJ14" s="48"/>
-      <c r="BK14" s="48"/>
-      <c r="BL14" s="49"/>
-      <c r="BM14" s="48"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="47"/>
+      <c r="O14" s="47"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47"/>
+      <c r="S14" s="47"/>
+      <c r="T14" s="47"/>
+      <c r="U14" s="47"/>
+      <c r="V14" s="47"/>
+      <c r="W14" s="46"/>
+      <c r="X14" s="47"/>
+      <c r="Y14" s="47"/>
+      <c r="Z14" s="46"/>
+      <c r="AA14" s="46"/>
+      <c r="AB14" s="46"/>
+      <c r="AC14" s="46"/>
+      <c r="AD14" s="46"/>
+      <c r="AE14" s="47"/>
+      <c r="AF14" s="47"/>
+      <c r="AG14" s="46"/>
+      <c r="AH14" s="46"/>
+      <c r="AI14" s="46"/>
+      <c r="AJ14" s="46"/>
+      <c r="AK14" s="46"/>
+      <c r="AL14" s="47"/>
+      <c r="AM14" s="47"/>
+      <c r="AN14" s="46"/>
+      <c r="AO14" s="46"/>
+      <c r="AP14" s="46"/>
+      <c r="AQ14" s="46"/>
+      <c r="AR14" s="46"/>
+      <c r="AS14" s="47"/>
+      <c r="AT14" s="47"/>
+      <c r="AU14" s="46"/>
+      <c r="AV14" s="46"/>
+      <c r="AW14" s="46"/>
+      <c r="AX14" s="46"/>
+      <c r="AY14" s="48"/>
+      <c r="AZ14" s="47"/>
+      <c r="BA14" s="47"/>
+      <c r="BB14" s="47"/>
+      <c r="BC14" s="47"/>
+      <c r="BD14" s="47"/>
+      <c r="BE14" s="47"/>
+      <c r="BF14" s="48"/>
+      <c r="BG14" s="47"/>
+      <c r="BH14" s="47"/>
+      <c r="BJ14" s="47"/>
+      <c r="BK14" s="47"/>
+      <c r="BL14" s="48"/>
+      <c r="BM14" s="47"/>
       <c r="BN14" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6102,75 +6097,75 @@
         <f aca="false">Netzplan!I13</f>
         <v>1</v>
       </c>
-      <c r="J15" s="45" t="n">
+      <c r="J15" s="44" t="n">
         <f aca="false">Netzplan!J13</f>
         <v>3</v>
       </c>
-      <c r="K15" s="46" t="n">
+      <c r="K15" s="45" t="n">
         <f aca="false">SUM(L15:BM15)</f>
         <v>3</v>
       </c>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="48"/>
-      <c r="S15" s="48"/>
-      <c r="T15" s="48"/>
-      <c r="U15" s="48"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="48"/>
-      <c r="X15" s="48"/>
-      <c r="Y15" s="48"/>
-      <c r="Z15" s="48"/>
-      <c r="AA15" s="48"/>
-      <c r="AB15" s="48"/>
-      <c r="AC15" s="48"/>
-      <c r="AD15" s="48"/>
-      <c r="AE15" s="48"/>
-      <c r="AF15" s="48"/>
-      <c r="AG15" s="48"/>
-      <c r="AH15" s="48"/>
-      <c r="AI15" s="48"/>
-      <c r="AJ15" s="48"/>
-      <c r="AL15" s="48"/>
-      <c r="AM15" s="48"/>
-      <c r="AN15" s="47"/>
-      <c r="AO15" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP15" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ15" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR15" s="48"/>
-      <c r="AS15" s="48"/>
-      <c r="AT15" s="48"/>
-      <c r="AU15" s="48"/>
-      <c r="AV15" s="48"/>
-      <c r="AW15" s="48"/>
-      <c r="AX15" s="48"/>
-      <c r="AY15" s="49"/>
-      <c r="AZ15" s="48"/>
-      <c r="BA15" s="48"/>
-      <c r="BB15" s="48"/>
-      <c r="BC15" s="48"/>
-      <c r="BD15" s="48"/>
-      <c r="BE15" s="48"/>
-      <c r="BF15" s="49"/>
-      <c r="BG15" s="48"/>
-      <c r="BH15" s="48"/>
-      <c r="BI15" s="48"/>
-      <c r="BJ15" s="48"/>
-      <c r="BK15" s="48"/>
-      <c r="BL15" s="49"/>
-      <c r="BM15" s="48"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="47"/>
+      <c r="V15" s="47"/>
+      <c r="W15" s="47"/>
+      <c r="X15" s="47"/>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="47"/>
+      <c r="AA15" s="47"/>
+      <c r="AB15" s="47"/>
+      <c r="AC15" s="47"/>
+      <c r="AD15" s="47"/>
+      <c r="AE15" s="47"/>
+      <c r="AF15" s="47"/>
+      <c r="AG15" s="47"/>
+      <c r="AH15" s="47"/>
+      <c r="AI15" s="47"/>
+      <c r="AJ15" s="47"/>
+      <c r="AL15" s="47"/>
+      <c r="AM15" s="47"/>
+      <c r="AN15" s="46"/>
+      <c r="AO15" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ15" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR15" s="47"/>
+      <c r="AS15" s="47"/>
+      <c r="AT15" s="47"/>
+      <c r="AU15" s="47"/>
+      <c r="AV15" s="47"/>
+      <c r="AW15" s="47"/>
+      <c r="AX15" s="47"/>
+      <c r="AY15" s="48"/>
+      <c r="AZ15" s="47"/>
+      <c r="BA15" s="47"/>
+      <c r="BB15" s="47"/>
+      <c r="BC15" s="47"/>
+      <c r="BD15" s="47"/>
+      <c r="BE15" s="47"/>
+      <c r="BF15" s="48"/>
+      <c r="BG15" s="47"/>
+      <c r="BH15" s="47"/>
+      <c r="BI15" s="47"/>
+      <c r="BJ15" s="47"/>
+      <c r="BK15" s="47"/>
+      <c r="BL15" s="48"/>
+      <c r="BM15" s="47"/>
       <c r="BN15" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6200,81 +6195,81 @@
         <f aca="false">Netzplan!I14</f>
         <v>1</v>
       </c>
-      <c r="J16" s="45" t="n">
+      <c r="J16" s="44" t="n">
         <f aca="false">Netzplan!J14</f>
         <v>3</v>
       </c>
-      <c r="K16" s="46" t="n">
+      <c r="K16" s="45" t="n">
         <f aca="false">SUM(L16:BM16)</f>
         <v>3</v>
       </c>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="48"/>
-      <c r="R16" s="48"/>
-      <c r="S16" s="48"/>
-      <c r="T16" s="48"/>
-      <c r="U16" s="48"/>
-      <c r="V16" s="48"/>
-      <c r="W16" s="48"/>
-      <c r="X16" s="48"/>
-      <c r="Y16" s="48"/>
-      <c r="Z16" s="48"/>
-      <c r="AA16" s="48"/>
-      <c r="AB16" s="48"/>
-      <c r="AC16" s="48"/>
-      <c r="AD16" s="48"/>
-      <c r="AE16" s="48"/>
-      <c r="AF16" s="48"/>
-      <c r="AG16" s="48"/>
-      <c r="AH16" s="48"/>
-      <c r="AI16" s="48"/>
-      <c r="AJ16" s="48"/>
-      <c r="AK16" s="48"/>
-      <c r="AL16" s="48"/>
-      <c r="AM16" s="48"/>
-      <c r="AN16" s="48"/>
-      <c r="AO16" s="48"/>
-      <c r="AQ16" s="47"/>
-      <c r="AR16" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS16" s="48"/>
-      <c r="AT16" s="48"/>
-      <c r="AU16" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV16" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW16" s="48"/>
-      <c r="AX16" s="48"/>
-      <c r="AY16" s="49"/>
-      <c r="AZ16" s="48"/>
-      <c r="BA16" s="48"/>
-      <c r="BB16" s="48"/>
-      <c r="BC16" s="48"/>
-      <c r="BD16" s="48"/>
-      <c r="BE16" s="48"/>
-      <c r="BF16" s="49"/>
-      <c r="BG16" s="48"/>
-      <c r="BH16" s="48"/>
-      <c r="BI16" s="48"/>
-      <c r="BJ16" s="48"/>
-      <c r="BK16" s="48"/>
-      <c r="BL16" s="49"/>
-      <c r="BM16" s="48"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="47"/>
+      <c r="V16" s="47"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="47"/>
+      <c r="Y16" s="47"/>
+      <c r="Z16" s="47"/>
+      <c r="AA16" s="47"/>
+      <c r="AB16" s="47"/>
+      <c r="AC16" s="47"/>
+      <c r="AD16" s="47"/>
+      <c r="AE16" s="47"/>
+      <c r="AF16" s="47"/>
+      <c r="AG16" s="47"/>
+      <c r="AH16" s="47"/>
+      <c r="AI16" s="47"/>
+      <c r="AJ16" s="47"/>
+      <c r="AK16" s="47"/>
+      <c r="AL16" s="47"/>
+      <c r="AM16" s="47"/>
+      <c r="AN16" s="47"/>
+      <c r="AO16" s="47"/>
+      <c r="AQ16" s="46"/>
+      <c r="AR16" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS16" s="47"/>
+      <c r="AT16" s="47"/>
+      <c r="AU16" s="46" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV16" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW16" s="47"/>
+      <c r="AX16" s="47"/>
+      <c r="AY16" s="48"/>
+      <c r="AZ16" s="47"/>
+      <c r="BA16" s="47"/>
+      <c r="BB16" s="47"/>
+      <c r="BC16" s="47"/>
+      <c r="BD16" s="47"/>
+      <c r="BE16" s="47"/>
+      <c r="BF16" s="48"/>
+      <c r="BG16" s="47"/>
+      <c r="BH16" s="47"/>
+      <c r="BI16" s="47"/>
+      <c r="BJ16" s="47"/>
+      <c r="BK16" s="47"/>
+      <c r="BL16" s="48"/>
+      <c r="BM16" s="47"/>
       <c r="BN16" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="14"/>
       <c r="B17" s="36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="36"/>
       <c r="D17" s="36"/>
@@ -6283,63 +6278,63 @@
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
       <c r="I17" s="31"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="48"/>
-      <c r="M17" s="48"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="48"/>
-      <c r="P17" s="48"/>
-      <c r="Q17" s="48"/>
-      <c r="R17" s="48"/>
-      <c r="S17" s="48"/>
-      <c r="T17" s="48"/>
-      <c r="U17" s="48"/>
-      <c r="V17" s="48"/>
-      <c r="W17" s="48"/>
-      <c r="X17" s="48"/>
-      <c r="Y17" s="48"/>
-      <c r="Z17" s="48"/>
-      <c r="AA17" s="48"/>
-      <c r="AB17" s="48"/>
-      <c r="AC17" s="48"/>
-      <c r="AD17" s="48"/>
-      <c r="AE17" s="48"/>
-      <c r="AF17" s="48"/>
-      <c r="AG17" s="48"/>
-      <c r="AH17" s="48"/>
-      <c r="AI17" s="48"/>
-      <c r="AJ17" s="48"/>
-      <c r="AK17" s="48"/>
-      <c r="AL17" s="48"/>
-      <c r="AM17" s="48"/>
-      <c r="AN17" s="48"/>
-      <c r="AO17" s="48"/>
-      <c r="AQ17" s="47"/>
-      <c r="AR17" s="47"/>
-      <c r="AS17" s="48"/>
-      <c r="AT17" s="48"/>
-      <c r="AU17" s="47"/>
-      <c r="AV17" s="48"/>
-      <c r="AW17" s="48"/>
-      <c r="AX17" s="48"/>
-      <c r="AY17" s="49"/>
-      <c r="AZ17" s="48"/>
-      <c r="BA17" s="48"/>
-      <c r="BB17" s="48"/>
-      <c r="BC17" s="48"/>
-      <c r="BD17" s="48"/>
-      <c r="BE17" s="48"/>
-      <c r="BF17" s="49"/>
-      <c r="BG17" s="48"/>
-      <c r="BH17" s="48"/>
-      <c r="BI17" s="48"/>
-      <c r="BJ17" s="48"/>
-      <c r="BK17" s="48"/>
-      <c r="BL17" s="49"/>
-      <c r="BM17" s="48"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="47"/>
+      <c r="AA17" s="47"/>
+      <c r="AB17" s="47"/>
+      <c r="AC17" s="47"/>
+      <c r="AD17" s="47"/>
+      <c r="AE17" s="47"/>
+      <c r="AF17" s="47"/>
+      <c r="AG17" s="47"/>
+      <c r="AH17" s="47"/>
+      <c r="AI17" s="47"/>
+      <c r="AJ17" s="47"/>
+      <c r="AK17" s="47"/>
+      <c r="AL17" s="47"/>
+      <c r="AM17" s="47"/>
+      <c r="AN17" s="47"/>
+      <c r="AO17" s="47"/>
+      <c r="AQ17" s="46"/>
+      <c r="AR17" s="46"/>
+      <c r="AS17" s="47"/>
+      <c r="AT17" s="47"/>
+      <c r="AU17" s="46"/>
+      <c r="AV17" s="47"/>
+      <c r="AW17" s="47"/>
+      <c r="AX17" s="47"/>
+      <c r="AY17" s="48"/>
+      <c r="AZ17" s="47"/>
+      <c r="BA17" s="47"/>
+      <c r="BB17" s="47"/>
+      <c r="BC17" s="47"/>
+      <c r="BD17" s="47"/>
+      <c r="BE17" s="47"/>
+      <c r="BF17" s="48"/>
+      <c r="BG17" s="47"/>
+      <c r="BH17" s="47"/>
+      <c r="BI17" s="47"/>
+      <c r="BJ17" s="47"/>
+      <c r="BK17" s="47"/>
+      <c r="BL17" s="48"/>
+      <c r="BM17" s="47"/>
       <c r="BN17" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6369,72 +6364,72 @@
         <f aca="false">Netzplan!I15</f>
         <v>1</v>
       </c>
-      <c r="J18" s="45" t="n">
+      <c r="J18" s="44" t="n">
         <f aca="false">Netzplan!J15</f>
         <v>1</v>
       </c>
-      <c r="K18" s="46" t="n">
+      <c r="K18" s="45" t="n">
         <f aca="false">SUM(L18:BM18)</f>
         <v>1</v>
       </c>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="48"/>
-      <c r="O18" s="48"/>
-      <c r="P18" s="48"/>
-      <c r="Q18" s="48"/>
-      <c r="R18" s="48"/>
-      <c r="S18" s="48"/>
-      <c r="T18" s="48"/>
-      <c r="U18" s="48"/>
-      <c r="V18" s="48"/>
-      <c r="W18" s="48"/>
-      <c r="X18" s="48"/>
-      <c r="Y18" s="48"/>
-      <c r="Z18" s="48"/>
-      <c r="AA18" s="48"/>
-      <c r="AB18" s="48"/>
-      <c r="AC18" s="48"/>
-      <c r="AD18" s="48"/>
-      <c r="AE18" s="48"/>
-      <c r="AF18" s="48"/>
-      <c r="AG18" s="48"/>
-      <c r="AH18" s="48"/>
-      <c r="AI18" s="48"/>
-      <c r="AJ18" s="48"/>
-      <c r="AK18" s="48"/>
-      <c r="AL18" s="48"/>
-      <c r="AM18" s="48"/>
-      <c r="AN18" s="48"/>
-      <c r="AO18" s="48"/>
-      <c r="AP18" s="48"/>
-      <c r="AQ18" s="48"/>
-      <c r="AR18" s="48"/>
-      <c r="AS18" s="48"/>
-      <c r="AT18" s="48"/>
-      <c r="AU18" s="48"/>
-      <c r="AV18" s="47"/>
-      <c r="AW18" s="48"/>
-      <c r="AX18" s="48"/>
-      <c r="AY18" s="49"/>
-      <c r="AZ18" s="48"/>
-      <c r="BA18" s="48"/>
-      <c r="BB18" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC18" s="48"/>
-      <c r="BD18" s="48"/>
-      <c r="BE18" s="48"/>
-      <c r="BF18" s="49"/>
-      <c r="BG18" s="48"/>
-      <c r="BH18" s="48"/>
-      <c r="BI18" s="48"/>
-      <c r="BJ18" s="48"/>
-      <c r="BK18" s="48"/>
-      <c r="BL18" s="49"/>
-      <c r="BM18" s="48"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="47"/>
+      <c r="R18" s="47"/>
+      <c r="S18" s="47"/>
+      <c r="T18" s="47"/>
+      <c r="U18" s="47"/>
+      <c r="V18" s="47"/>
+      <c r="W18" s="47"/>
+      <c r="X18" s="47"/>
+      <c r="Y18" s="47"/>
+      <c r="Z18" s="47"/>
+      <c r="AA18" s="47"/>
+      <c r="AB18" s="47"/>
+      <c r="AC18" s="47"/>
+      <c r="AD18" s="47"/>
+      <c r="AE18" s="47"/>
+      <c r="AF18" s="47"/>
+      <c r="AG18" s="47"/>
+      <c r="AH18" s="47"/>
+      <c r="AI18" s="47"/>
+      <c r="AJ18" s="47"/>
+      <c r="AK18" s="47"/>
+      <c r="AL18" s="47"/>
+      <c r="AM18" s="47"/>
+      <c r="AN18" s="47"/>
+      <c r="AO18" s="47"/>
+      <c r="AP18" s="47"/>
+      <c r="AQ18" s="47"/>
+      <c r="AR18" s="47"/>
+      <c r="AS18" s="47"/>
+      <c r="AT18" s="47"/>
+      <c r="AU18" s="47"/>
+      <c r="AV18" s="46"/>
+      <c r="AW18" s="47"/>
+      <c r="AX18" s="47"/>
+      <c r="AY18" s="48"/>
+      <c r="AZ18" s="47"/>
+      <c r="BA18" s="47"/>
+      <c r="BB18" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC18" s="47"/>
+      <c r="BD18" s="47"/>
+      <c r="BE18" s="47"/>
+      <c r="BF18" s="48"/>
+      <c r="BG18" s="47"/>
+      <c r="BH18" s="47"/>
+      <c r="BI18" s="47"/>
+      <c r="BJ18" s="47"/>
+      <c r="BK18" s="47"/>
+      <c r="BL18" s="48"/>
+      <c r="BM18" s="47"/>
       <c r="BN18" s="0" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6458,81 +6453,81 @@
       </c>
       <c r="H19" s="30" t="str">
         <f aca="false">Netzplan!H16</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" s="31" t="n">
         <f aca="false">Netzplan!I16</f>
-        <v>0.75</v>
-      </c>
-      <c r="J19" s="45" t="n">
+        <v>1</v>
+      </c>
+      <c r="J19" s="44" t="n">
         <f aca="false">Netzplan!J16</f>
-        <v>3</v>
-      </c>
-      <c r="K19" s="46" t="n">
+        <v>5</v>
+      </c>
+      <c r="K19" s="45" t="n">
         <f aca="false">SUM(L19:BM19)</f>
         <v>3</v>
       </c>
-      <c r="L19" s="48"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="48"/>
-      <c r="P19" s="48"/>
-      <c r="Q19" s="48"/>
-      <c r="R19" s="48"/>
-      <c r="S19" s="48"/>
-      <c r="T19" s="48"/>
-      <c r="U19" s="48"/>
-      <c r="V19" s="48"/>
-      <c r="W19" s="48"/>
-      <c r="X19" s="48"/>
-      <c r="Y19" s="48"/>
-      <c r="Z19" s="48"/>
-      <c r="AA19" s="48"/>
-      <c r="AB19" s="48"/>
-      <c r="AC19" s="48"/>
-      <c r="AD19" s="48"/>
-      <c r="AE19" s="48"/>
-      <c r="AF19" s="48"/>
-      <c r="AG19" s="48"/>
-      <c r="AH19" s="48"/>
-      <c r="AI19" s="48"/>
-      <c r="AJ19" s="48"/>
-      <c r="AK19" s="48"/>
-      <c r="AL19" s="48"/>
-      <c r="AM19" s="48"/>
-      <c r="AN19" s="48"/>
-      <c r="AO19" s="48"/>
-      <c r="AP19" s="48"/>
-      <c r="AQ19" s="48"/>
-      <c r="AR19" s="48"/>
-      <c r="AS19" s="48"/>
-      <c r="AT19" s="48"/>
-      <c r="AU19" s="48"/>
-      <c r="AV19" s="48"/>
-      <c r="AW19" s="47"/>
-      <c r="AX19" s="47"/>
-      <c r="AY19" s="49"/>
-      <c r="AZ19" s="48"/>
-      <c r="BA19" s="48"/>
-      <c r="BB19" s="47"/>
-      <c r="BC19" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD19" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="BE19" s="48" t="n">
-        <v>1</v>
-      </c>
-      <c r="BF19" s="49"/>
-      <c r="BG19" s="48"/>
-      <c r="BH19" s="48"/>
-      <c r="BI19" s="48"/>
-      <c r="BK19" s="48"/>
-      <c r="BL19" s="49"/>
-      <c r="BM19" s="48"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="47"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="47"/>
+      <c r="R19" s="47"/>
+      <c r="S19" s="47"/>
+      <c r="T19" s="47"/>
+      <c r="U19" s="47"/>
+      <c r="V19" s="47"/>
+      <c r="W19" s="47"/>
+      <c r="X19" s="47"/>
+      <c r="Y19" s="47"/>
+      <c r="Z19" s="47"/>
+      <c r="AA19" s="47"/>
+      <c r="AB19" s="47"/>
+      <c r="AC19" s="47"/>
+      <c r="AD19" s="47"/>
+      <c r="AE19" s="47"/>
+      <c r="AF19" s="47"/>
+      <c r="AG19" s="47"/>
+      <c r="AH19" s="47"/>
+      <c r="AI19" s="47"/>
+      <c r="AJ19" s="47"/>
+      <c r="AK19" s="47"/>
+      <c r="AL19" s="47"/>
+      <c r="AM19" s="47"/>
+      <c r="AN19" s="47"/>
+      <c r="AO19" s="47"/>
+      <c r="AP19" s="47"/>
+      <c r="AQ19" s="47"/>
+      <c r="AR19" s="47"/>
+      <c r="AS19" s="47"/>
+      <c r="AT19" s="47"/>
+      <c r="AU19" s="47"/>
+      <c r="AV19" s="47"/>
+      <c r="AW19" s="46"/>
+      <c r="AX19" s="46"/>
+      <c r="AY19" s="48"/>
+      <c r="AZ19" s="47"/>
+      <c r="BA19" s="47"/>
+      <c r="BB19" s="46"/>
+      <c r="BC19" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD19" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE19" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF19" s="48"/>
+      <c r="BG19" s="47"/>
+      <c r="BH19" s="47"/>
+      <c r="BI19" s="47"/>
+      <c r="BK19" s="47"/>
+      <c r="BL19" s="48"/>
+      <c r="BM19" s="47"/>
       <c r="BN19" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6545,7 +6540,7 @@
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" s="38"/>
       <c r="G20" s="39" t="n">
@@ -6556,7 +6551,7 @@
         <f aca="false">Netzplan!H17</f>
         <v>1</v>
       </c>
-      <c r="I20" s="40" t="n">
+      <c r="I20" s="51" t="n">
         <f aca="false">Netzplan!I17</f>
         <v>1</v>
       </c>
@@ -6564,7 +6559,7 @@
         <f aca="false">Netzplan!J17</f>
         <v>1</v>
       </c>
-      <c r="K20" s="46" t="n">
+      <c r="K20" s="45" t="n">
         <f aca="false">SUM(L20:BM20)</f>
         <v>1</v>
       </c>
@@ -6611,7 +6606,7 @@
       <c r="AZ20" s="53"/>
       <c r="BA20" s="53"/>
       <c r="BB20" s="53"/>
-      <c r="BC20" s="47"/>
+      <c r="BC20" s="46"/>
       <c r="BD20" s="53"/>
       <c r="BE20" s="53"/>
       <c r="BF20" s="54"/>
@@ -6625,7 +6620,7 @@
       <c r="BL20" s="54"/>
       <c r="BM20" s="53"/>
       <c r="BN20" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>